<commit_message>
Change to create 2 layers of ref portfolio
</commit_message>
<xml_diff>
--- a/examples/use-cases/valuation/data/lookthrough_data.xlsx
+++ b/examples/use-cases/valuation/data/lookthrough_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ThomasPartridge\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AndrewPoulter\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{065B1F0A-A63E-48F1-B2EF-147DCEF9317B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBE33215-F025-4C51-8363-D3E1CEAE9E90}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="12852" windowWidth="23256" windowHeight="14016" xr2:uid="{140D0F4F-AA5F-4E16-95A8-8F9F58C5F424}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{140D0F4F-AA5F-4E16-95A8-8F9F58C5F424}"/>
   </bookViews>
   <sheets>
     <sheet name="transactions" sheetId="3" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="520" uniqueCount="156">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="540" uniqueCount="160">
   <si>
     <t>date</t>
   </si>
@@ -505,6 +505,18 @@
   </si>
   <si>
     <t>cash_id</t>
+  </si>
+  <si>
+    <t>txnid_0021</t>
+  </si>
+  <si>
+    <t>USEquityFinancials Fund</t>
+  </si>
+  <si>
+    <t>fund_USEquityFinancials</t>
+  </si>
+  <si>
+    <t>USEquityFinancials</t>
   </si>
 </sst>
 </file>
@@ -557,12 +569,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -888,22 +895,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33E4483A-D81C-486B-9469-6BB1913F7014}">
-  <dimension ref="A1:L21"/>
+  <dimension ref="A1:L22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L23" sqref="L23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.85546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="19.85546875" style="3" customWidth="1"/>
-    <col min="6" max="6" width="22.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="19.85546875" customWidth="1"/>
+    <col min="6" max="6" width="26.7109375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="13.28515625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="28.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="18.42578125" style="3" customWidth="1"/>
+    <col min="9" max="9" width="18.42578125" customWidth="1"/>
     <col min="10" max="10" width="8.5703125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="12" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="18.5703125" bestFit="1" customWidth="1"/>
@@ -911,741 +918,780 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+      <c r="A1" t="s">
         <v>90</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="F1" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="G1" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="H1" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="I1" s="1" t="s">
         <v>155</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="J1" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="K1" s="4" t="s">
+      <c r="K1" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="L1" s="4" t="s">
+      <c r="L1" s="1" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+      <c r="A2" t="s">
         <v>93</v>
       </c>
-      <c r="B2" s="5" t="s">
-        <v>107</v>
-      </c>
-      <c r="C2" s="5" t="s">
+      <c r="B2" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="D2" s="5" t="s">
-        <v>107</v>
-      </c>
-      <c r="E2" s="5" t="s">
-        <v>108</v>
-      </c>
-      <c r="F2" s="3" t="s">
+      <c r="D2" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="F2" t="s">
         <v>64</v>
       </c>
-      <c r="G2" s="4">
+      <c r="G2" s="1">
         <v>2000</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="H2" t="s">
         <v>75</v>
       </c>
-      <c r="J2" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="K2" s="3">
+      <c r="J2" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="K2">
         <v>145.9</v>
       </c>
-      <c r="L2" s="3">
+      <c r="L2">
         <v>291800</v>
       </c>
     </row>
-    <row r="3" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>94</v>
       </c>
-      <c r="B3" s="5" t="s">
-        <v>107</v>
-      </c>
-      <c r="C3" s="5" t="s">
+      <c r="B3" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="D3" s="5" t="s">
-        <v>107</v>
-      </c>
-      <c r="E3" s="5" t="s">
-        <v>108</v>
-      </c>
-      <c r="F3" s="3" t="s">
+      <c r="D3" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="F3" t="s">
         <v>64</v>
       </c>
-      <c r="G3" s="4">
+      <c r="G3" s="1">
         <v>500</v>
       </c>
-      <c r="H3" s="3" t="s">
+      <c r="H3" t="s">
         <v>76</v>
       </c>
-      <c r="J3" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="K3" s="3">
+      <c r="J3" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="K3">
         <v>179.63</v>
       </c>
-      <c r="L3" s="3">
+      <c r="L3">
         <v>89815</v>
       </c>
     </row>
-    <row r="4" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>95</v>
       </c>
-      <c r="B4" s="5" t="s">
-        <v>107</v>
-      </c>
-      <c r="C4" s="5" t="s">
+      <c r="B4" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="D4" s="5" t="s">
-        <v>107</v>
-      </c>
-      <c r="E4" s="5" t="s">
-        <v>108</v>
-      </c>
-      <c r="F4" s="3" t="s">
+      <c r="D4" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="F4" t="s">
         <v>64</v>
       </c>
-      <c r="G4" s="4">
+      <c r="G4" s="1">
         <v>750</v>
       </c>
-      <c r="H4" s="3" t="s">
+      <c r="H4" t="s">
         <v>77</v>
       </c>
-      <c r="J4" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="K4" s="3">
+      <c r="J4" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="K4">
         <v>120.05</v>
       </c>
-      <c r="L4" s="3">
+      <c r="L4">
         <v>90037.5</v>
       </c>
     </row>
-    <row r="5" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>96</v>
       </c>
-      <c r="B5" s="5" t="s">
-        <v>107</v>
-      </c>
-      <c r="C5" s="5" t="s">
+      <c r="B5" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="C5" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="D5" s="5" t="s">
-        <v>107</v>
-      </c>
-      <c r="E5" s="5" t="s">
-        <v>108</v>
-      </c>
-      <c r="F5" s="3" t="s">
+      <c r="D5" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="F5" t="s">
         <v>64</v>
       </c>
-      <c r="G5" s="4">
+      <c r="G5" s="1">
         <v>100</v>
       </c>
-      <c r="H5" s="3" t="s">
+      <c r="H5" t="s">
         <v>87</v>
       </c>
-      <c r="J5" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="K5" s="3">
+      <c r="J5" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="K5">
         <v>7469.99</v>
       </c>
-      <c r="L5" s="3">
+      <c r="L5">
         <v>746999</v>
       </c>
     </row>
-    <row r="6" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>97</v>
       </c>
-      <c r="B6" s="5" t="s">
-        <v>107</v>
-      </c>
-      <c r="C6" s="5" t="s">
+      <c r="B6" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="C6" s="2" t="s">
         <v>154</v>
       </c>
-      <c r="D6" s="5" t="s">
-        <v>107</v>
-      </c>
-      <c r="E6" s="5" t="s">
-        <v>108</v>
-      </c>
-      <c r="F6" s="3" t="s">
+      <c r="D6" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="F6" t="s">
         <v>64</v>
       </c>
-      <c r="G6" s="4">
+      <c r="G6" s="1">
         <v>1300000</v>
       </c>
-      <c r="I6" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="J6" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="K6" s="3">
+      <c r="I6" t="s">
+        <v>56</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="K6">
         <v>1</v>
       </c>
-      <c r="L6" s="3">
+      <c r="L6">
         <v>1300000</v>
       </c>
     </row>
-    <row r="7" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>98</v>
       </c>
-      <c r="B7" s="5" t="s">
-        <v>107</v>
-      </c>
-      <c r="C7" s="5" t="s">
+      <c r="B7" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="C7" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="D7" s="5" t="s">
-        <v>107</v>
-      </c>
-      <c r="E7" s="5" t="s">
-        <v>108</v>
-      </c>
-      <c r="F7" s="3" t="s">
+      <c r="D7" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="F7" t="s">
         <v>62</v>
       </c>
-      <c r="G7" s="4">
+      <c r="G7" s="1">
         <v>5000</v>
       </c>
-      <c r="H7" s="3" t="s">
+      <c r="H7" t="s">
         <v>80</v>
       </c>
-      <c r="J7" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="K7" s="3">
+      <c r="J7" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="K7">
         <v>29.01</v>
       </c>
-      <c r="L7" s="3">
+      <c r="L7">
         <v>145050</v>
       </c>
     </row>
-    <row r="8" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>99</v>
       </c>
-      <c r="B8" s="5" t="s">
-        <v>107</v>
-      </c>
-      <c r="C8" s="5" t="s">
+      <c r="B8" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="C8" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="D8" s="5" t="s">
-        <v>107</v>
-      </c>
-      <c r="E8" s="5" t="s">
-        <v>108</v>
-      </c>
-      <c r="F8" s="3" t="s">
+      <c r="D8" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="F8" t="s">
         <v>62</v>
       </c>
-      <c r="G8" s="4">
+      <c r="G8" s="1">
         <v>750</v>
       </c>
-      <c r="H8" s="3" t="s">
+      <c r="H8" t="s">
         <v>78</v>
       </c>
-      <c r="J8" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="K8" s="3">
+      <c r="J8" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="K8">
         <v>65.819999999999993</v>
       </c>
-      <c r="L8" s="3">
+      <c r="L8">
         <v>49364.999999999993</v>
       </c>
     </row>
-    <row r="9" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="3" t="s">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
         <v>100</v>
       </c>
-      <c r="B9" s="5" t="s">
-        <v>107</v>
-      </c>
-      <c r="C9" s="5" t="s">
+      <c r="B9" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="C9" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="D9" s="5" t="s">
-        <v>107</v>
-      </c>
-      <c r="E9" s="5" t="s">
-        <v>108</v>
-      </c>
-      <c r="F9" s="3" t="s">
+      <c r="D9" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="F9" t="s">
         <v>62</v>
       </c>
-      <c r="G9" s="4">
+      <c r="G9" s="1">
         <v>3000</v>
       </c>
-      <c r="H9" s="3" t="s">
+      <c r="H9" t="s">
         <v>79</v>
       </c>
-      <c r="J9" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="K9" s="3">
+      <c r="J9" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="K9">
         <v>121.16</v>
       </c>
-      <c r="L9" s="3">
+      <c r="L9">
         <v>363480</v>
       </c>
     </row>
-    <row r="10" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="3" t="s">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
         <v>101</v>
       </c>
-      <c r="B10" s="5" t="s">
-        <v>107</v>
-      </c>
-      <c r="C10" s="5" t="s">
+      <c r="B10" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="C10" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="D10" s="5" t="s">
-        <v>107</v>
-      </c>
-      <c r="E10" s="5" t="s">
-        <v>108</v>
-      </c>
-      <c r="F10" s="3" t="s">
+      <c r="D10" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="F10" t="s">
         <v>62</v>
       </c>
-      <c r="G10" s="4">
+      <c r="G10" s="1">
         <v>1000</v>
       </c>
-      <c r="H10" s="3" t="s">
+      <c r="H10" t="s">
         <v>86</v>
       </c>
-      <c r="J10" s="4" t="s">
+      <c r="J10" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="K10" s="3">
+      <c r="K10">
         <v>32.840000000000003</v>
       </c>
-      <c r="L10" s="3">
+      <c r="L10">
         <v>32840</v>
       </c>
     </row>
-    <row r="11" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="3" t="s">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
         <v>102</v>
       </c>
-      <c r="B11" s="5" t="s">
-        <v>107</v>
-      </c>
-      <c r="C11" s="5" t="s">
+      <c r="B11" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="C11" s="2" t="s">
         <v>154</v>
       </c>
-      <c r="D11" s="5" t="s">
-        <v>107</v>
-      </c>
-      <c r="E11" s="5" t="s">
-        <v>108</v>
-      </c>
-      <c r="F11" s="3" t="s">
+      <c r="D11" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="F11" t="s">
         <v>62</v>
       </c>
-      <c r="G11" s="4">
+      <c r="G11" s="1">
         <v>700000</v>
       </c>
-      <c r="I11" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="J11" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="K11" s="3">
+      <c r="I11" t="s">
+        <v>56</v>
+      </c>
+      <c r="J11" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="K11">
         <v>1</v>
       </c>
-      <c r="L11" s="3">
+      <c r="L11">
         <v>700000</v>
       </c>
     </row>
-    <row r="12" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="3" t="s">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
         <v>103</v>
       </c>
-      <c r="B12" s="5" t="s">
-        <v>107</v>
-      </c>
-      <c r="C12" s="5" t="s">
+      <c r="B12" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="C12" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="D12" s="5" t="s">
-        <v>107</v>
-      </c>
-      <c r="E12" s="5" t="s">
-        <v>108</v>
-      </c>
-      <c r="F12" s="3" t="s">
+      <c r="D12" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="F12" t="s">
+        <v>159</v>
+      </c>
+      <c r="G12" s="1">
+        <v>250</v>
+      </c>
+      <c r="H12" t="s">
+        <v>81</v>
+      </c>
+      <c r="J12" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="K12">
+        <v>167.87</v>
+      </c>
+      <c r="L12">
+        <v>41967.5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>104</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="F13" t="s">
+        <v>159</v>
+      </c>
+      <c r="G13" s="1">
+        <v>1000</v>
+      </c>
+      <c r="H13" t="s">
+        <v>82</v>
+      </c>
+      <c r="J13" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="K13">
+        <v>64.25</v>
+      </c>
+      <c r="L13">
+        <v>64250</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>105</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="F14" t="s">
+        <v>159</v>
+      </c>
+      <c r="G14" s="1">
+        <v>100</v>
+      </c>
+      <c r="H14" t="s">
+        <v>83</v>
+      </c>
+      <c r="J14" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="K14">
+        <v>407.33</v>
+      </c>
+      <c r="L14">
+        <v>40733</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>118</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="F15" t="s">
         <v>63</v>
       </c>
-      <c r="G12" s="4">
-        <v>250</v>
-      </c>
-      <c r="H12" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="J12" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="K12" s="3">
-        <v>167.87</v>
-      </c>
-      <c r="L12" s="3">
-        <v>41967.5</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="3" t="s">
-        <v>104</v>
-      </c>
-      <c r="B13" s="5" t="s">
-        <v>107</v>
-      </c>
-      <c r="C13" s="5" t="s">
+      <c r="G15" s="1">
+        <v>5000</v>
+      </c>
+      <c r="H15" t="s">
+        <v>85</v>
+      </c>
+      <c r="J15" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="K15">
+        <v>137.22</v>
+      </c>
+      <c r="L15">
+        <v>686100</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>119</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="C16" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="D13" s="5" t="s">
-        <v>107</v>
-      </c>
-      <c r="E13" s="5" t="s">
-        <v>108</v>
-      </c>
-      <c r="F13" s="3" t="s">
+      <c r="D16" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="F16" t="s">
         <v>63</v>
       </c>
-      <c r="G13" s="4">
-        <v>1000</v>
-      </c>
-      <c r="H13" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="J13" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="K13" s="3">
-        <v>64.25</v>
-      </c>
-      <c r="L13" s="3">
-        <v>64250</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="3" t="s">
-        <v>105</v>
-      </c>
-      <c r="B14" s="5" t="s">
-        <v>107</v>
-      </c>
-      <c r="C14" s="5" t="s">
+      <c r="G16" s="1">
+        <v>350</v>
+      </c>
+      <c r="H16" t="s">
+        <v>84</v>
+      </c>
+      <c r="J16" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="K16">
+        <v>11.3</v>
+      </c>
+      <c r="L16">
+        <v>3955.0000000000005</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>120</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="F17" t="s">
+        <v>63</v>
+      </c>
+      <c r="G17" s="1">
+        <v>1000000</v>
+      </c>
+      <c r="I17" t="s">
+        <v>56</v>
+      </c>
+      <c r="J17" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="K17">
+        <v>1</v>
+      </c>
+      <c r="L17">
+        <v>1000000</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>150</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="C18" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="D14" s="5" t="s">
-        <v>107</v>
-      </c>
-      <c r="E14" s="5" t="s">
-        <v>108</v>
-      </c>
-      <c r="F14" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="G14" s="4">
-        <v>100</v>
-      </c>
-      <c r="H14" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="J14" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="K14" s="3">
-        <v>407.33</v>
-      </c>
-      <c r="L14" s="3">
-        <v>40733</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="3" t="s">
-        <v>118</v>
-      </c>
-      <c r="B15" s="5" t="s">
-        <v>107</v>
-      </c>
-      <c r="C15" s="5" t="s">
-        <v>92</v>
-      </c>
-      <c r="D15" s="5" t="s">
-        <v>107</v>
-      </c>
-      <c r="E15" s="5" t="s">
-        <v>108</v>
-      </c>
-      <c r="F15" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="G15" s="4">
-        <v>5000</v>
-      </c>
-      <c r="H15" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="J15" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="K15" s="3">
-        <v>137.22</v>
-      </c>
-      <c r="L15" s="3">
-        <v>686100</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="3" t="s">
-        <v>119</v>
-      </c>
-      <c r="B16" s="5" t="s">
-        <v>107</v>
-      </c>
-      <c r="C16" s="5" t="s">
-        <v>92</v>
-      </c>
-      <c r="D16" s="5" t="s">
-        <v>107</v>
-      </c>
-      <c r="E16" s="5" t="s">
-        <v>108</v>
-      </c>
-      <c r="F16" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="G16" s="4">
-        <v>350</v>
-      </c>
-      <c r="H16" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="J16" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="K16" s="3">
-        <v>11.3</v>
-      </c>
-      <c r="L16" s="3">
-        <v>3955.0000000000005</v>
-      </c>
-    </row>
-    <row r="17" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="3" t="s">
-        <v>120</v>
-      </c>
-      <c r="B17" s="5" t="s">
-        <v>107</v>
-      </c>
-      <c r="C17" s="5" t="s">
-        <v>154</v>
-      </c>
-      <c r="D17" s="5" t="s">
-        <v>107</v>
-      </c>
-      <c r="E17" s="5" t="s">
-        <v>108</v>
-      </c>
-      <c r="F17" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="G17" s="4">
-        <v>1000000</v>
-      </c>
-      <c r="I17" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="J17" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="K17" s="3">
-        <v>1</v>
-      </c>
-      <c r="L17" s="3">
-        <v>1000000</v>
-      </c>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A18" s="3" t="s">
-        <v>150</v>
-      </c>
-      <c r="B18" s="5" t="s">
-        <v>107</v>
-      </c>
-      <c r="C18" s="5" t="s">
-        <v>92</v>
-      </c>
-      <c r="D18" s="5" t="s">
-        <v>107</v>
-      </c>
-      <c r="E18" s="5" t="s">
-        <v>108</v>
-      </c>
-      <c r="F18" s="3" t="s">
+      <c r="D18" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="F18" t="s">
         <v>117</v>
       </c>
-      <c r="G18" s="4">
+      <c r="G18" s="1">
         <v>50</v>
       </c>
-      <c r="H18" s="3" t="s">
+      <c r="H18" t="s">
         <v>114</v>
       </c>
-      <c r="J18" s="4" t="s">
+      <c r="J18" s="1" t="s">
         <v>56</v>
       </c>
       <c r="K18">
         <v>119.5</v>
       </c>
-      <c r="L18" s="3">
+      <c r="L18">
         <v>5975</v>
       </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A19" s="3" t="s">
+      <c r="A19" t="s">
         <v>151</v>
       </c>
-      <c r="B19" s="5" t="s">
-        <v>107</v>
-      </c>
-      <c r="C19" s="5" t="s">
+      <c r="B19" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="C19" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="D19" s="5" t="s">
-        <v>107</v>
-      </c>
-      <c r="E19" s="5" t="s">
-        <v>108</v>
-      </c>
-      <c r="F19" s="3" t="s">
+      <c r="D19" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="F19" t="s">
         <v>117</v>
       </c>
-      <c r="G19" s="4">
+      <c r="G19" s="1">
         <v>50</v>
       </c>
-      <c r="H19" s="3" t="s">
+      <c r="H19" t="s">
         <v>115</v>
       </c>
-      <c r="J19" s="4" t="s">
+      <c r="J19" s="1" t="s">
         <v>56</v>
       </c>
       <c r="K19">
         <v>114</v>
       </c>
-      <c r="L19" s="3">
+      <c r="L19">
         <v>5700</v>
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A20" s="3" t="s">
+      <c r="A20" t="s">
         <v>152</v>
       </c>
-      <c r="B20" s="5" t="s">
-        <v>107</v>
-      </c>
-      <c r="C20" s="5" t="s">
+      <c r="B20" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="C20" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="D20" s="5" t="s">
-        <v>107</v>
-      </c>
-      <c r="E20" s="5" t="s">
-        <v>108</v>
-      </c>
-      <c r="F20" s="3" t="s">
+      <c r="D20" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="F20" t="s">
         <v>117</v>
       </c>
-      <c r="G20" s="4">
+      <c r="G20" s="1">
         <v>50</v>
       </c>
-      <c r="H20" s="3" t="s">
+      <c r="H20" t="s">
         <v>116</v>
       </c>
-      <c r="J20" s="4" t="s">
+      <c r="J20" s="1" t="s">
         <v>56</v>
       </c>
       <c r="K20">
         <v>96</v>
       </c>
-      <c r="L20" s="3">
+      <c r="L20">
         <v>4800</v>
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A21" s="3" t="s">
+      <c r="A21" t="s">
         <v>153</v>
       </c>
-      <c r="B21" s="5" t="s">
-        <v>107</v>
-      </c>
-      <c r="C21" s="5" t="s">
+      <c r="B21" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="C21" s="2" t="s">
         <v>154</v>
       </c>
-      <c r="D21" s="5" t="s">
-        <v>107</v>
-      </c>
-      <c r="E21" s="5" t="s">
-        <v>108</v>
-      </c>
-      <c r="F21" s="3" t="s">
+      <c r="D21" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="F21" t="s">
         <v>117</v>
       </c>
-      <c r="G21" s="4">
+      <c r="G21" s="1">
         <v>20000</v>
       </c>
-      <c r="I21" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="J21" s="4" t="s">
+      <c r="I21" t="s">
+        <v>56</v>
+      </c>
+      <c r="J21" s="1" t="s">
         <v>56</v>
       </c>
       <c r="K21">
         <v>1</v>
       </c>
-      <c r="L21" s="3">
+      <c r="L21">
         <v>20000</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>156</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="F22" t="s">
+        <v>63</v>
+      </c>
+      <c r="G22" s="1">
+        <v>25</v>
+      </c>
+      <c r="H22" t="s">
+        <v>158</v>
+      </c>
+      <c r="I22" t="s">
+        <v>56</v>
+      </c>
+      <c r="J22" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="K22">
+        <v>106</v>
+      </c>
+      <c r="L22">
+        <f>K22*G22</f>
+        <v>2650</v>
       </c>
     </row>
   </sheetData>
@@ -1665,7 +1711,7 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="7.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="17.85546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="7.140625" bestFit="1" customWidth="1"/>
@@ -1675,7 +1721,7 @@
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" t="s">
         <v>54</v>
       </c>
       <c r="C1" t="s">
@@ -1689,10 +1735,10 @@
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="s">
-        <v>108</v>
-      </c>
-      <c r="B2" s="2" t="s">
+      <c r="A2" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="B2" t="s">
         <v>57</v>
       </c>
       <c r="C2" t="s">
@@ -1706,10 +1752,10 @@
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="5" t="s">
-        <v>108</v>
-      </c>
-      <c r="B3" s="2" t="s">
+      <c r="A3" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="B3" t="s">
         <v>57</v>
       </c>
       <c r="C3" t="s">
@@ -1718,15 +1764,15 @@
       <c r="D3" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="E3" s="4">
+      <c r="E3" s="1">
         <v>0.1</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="5" t="s">
-        <v>108</v>
-      </c>
-      <c r="B4" s="2" t="s">
+      <c r="A4" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="B4" t="s">
         <v>57</v>
       </c>
       <c r="C4" t="s">
@@ -1735,15 +1781,15 @@
       <c r="D4" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="E4" s="4">
+      <c r="E4" s="1">
         <v>0.1</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="5" t="s">
-        <v>108</v>
-      </c>
-      <c r="B5" s="2" t="s">
+      <c r="A5" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="B5" t="s">
         <v>57</v>
       </c>
       <c r="C5" t="s">
@@ -1752,15 +1798,15 @@
       <c r="D5" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="E5" s="4">
+      <c r="E5" s="1">
         <v>0.1</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="5" t="s">
-        <v>108</v>
-      </c>
-      <c r="B6" s="2" t="s">
+      <c r="A6" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="B6" t="s">
         <v>57</v>
       </c>
       <c r="C6" t="s">
@@ -1769,15 +1815,15 @@
       <c r="D6" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="E6" s="4">
+      <c r="E6" s="1">
         <v>0.1</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="5" t="s">
-        <v>108</v>
-      </c>
-      <c r="B7" s="2" t="s">
+      <c r="A7" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="B7" t="s">
         <v>57</v>
       </c>
       <c r="C7" t="s">
@@ -1786,15 +1832,15 @@
       <c r="D7" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="E7" s="4">
+      <c r="E7" s="1">
         <v>0.1</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="5" t="s">
-        <v>108</v>
-      </c>
-      <c r="B8" s="2" t="s">
+      <c r="A8" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="B8" t="s">
         <v>57</v>
       </c>
       <c r="C8" t="s">
@@ -1803,15 +1849,15 @@
       <c r="D8" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="E8" s="4">
+      <c r="E8" s="1">
         <v>0.1</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="5" t="s">
-        <v>108</v>
-      </c>
-      <c r="B9" s="2" t="s">
+      <c r="A9" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="B9" t="s">
         <v>57</v>
       </c>
       <c r="C9" t="s">
@@ -1820,15 +1866,15 @@
       <c r="D9" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="E9" s="4">
+      <c r="E9" s="1">
         <v>0.1</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="5" t="s">
-        <v>108</v>
-      </c>
-      <c r="B10" s="2" t="s">
+      <c r="A10" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="B10" t="s">
         <v>57</v>
       </c>
       <c r="C10" t="s">
@@ -1837,15 +1883,15 @@
       <c r="D10" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="E10" s="4">
+      <c r="E10" s="1">
         <v>0.1</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="5" t="s">
-        <v>108</v>
-      </c>
-      <c r="B11" s="2" t="s">
+      <c r="A11" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="B11" t="s">
         <v>57</v>
       </c>
       <c r="C11" t="s">
@@ -1854,7 +1900,7 @@
       <c r="D11" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="E11" s="4">
+      <c r="E11" s="1">
         <v>0.1</v>
       </c>
     </row>
@@ -1867,431 +1913,420 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E615609-E297-47FD-9AAE-07E524F332F5}">
-  <dimension ref="A1:I28"/>
+  <dimension ref="A1:E29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A29" sqref="A29"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="27.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="6" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="8.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" t="s">
         <v>109</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" t="s">
         <v>110</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" t="s">
         <v>41</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="s">
-        <v>108</v>
-      </c>
-      <c r="B2" s="2" t="s">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="B2" t="s">
         <v>65</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" t="s">
         <v>111</v>
       </c>
-      <c r="D2" s="2">
+      <c r="D2">
         <v>146</v>
       </c>
-      <c r="E2" s="2" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="5" t="s">
-        <v>108</v>
-      </c>
-      <c r="B3" s="2" t="s">
+      <c r="E2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="B3" t="s">
         <v>66</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" t="s">
         <v>111</v>
       </c>
-      <c r="D3" s="2">
+      <c r="D3">
         <v>180</v>
       </c>
-      <c r="E3" s="2" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="5" t="s">
-        <v>108</v>
-      </c>
-      <c r="B4" s="2" t="s">
+      <c r="E3" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="B4" t="s">
         <v>67</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" t="s">
         <v>111</v>
       </c>
-      <c r="D4" s="2">
+      <c r="D4">
         <v>120</v>
       </c>
-      <c r="E4" s="2" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="5" t="s">
-        <v>108</v>
-      </c>
-      <c r="B5" s="2" t="s">
+      <c r="E4" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="B5" t="s">
         <v>68</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" t="s">
         <v>111</v>
       </c>
-      <c r="D5" s="2">
+      <c r="D5">
         <v>2888</v>
       </c>
-      <c r="E5" s="2" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="5" t="s">
-        <v>108</v>
-      </c>
-      <c r="B6" s="2" t="s">
+      <c r="E5" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="B6" t="s">
         <v>69</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C6" t="s">
         <v>111</v>
       </c>
-      <c r="D6" s="2">
+      <c r="D6">
         <v>329</v>
       </c>
-      <c r="E6" s="2" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="5" t="s">
-        <v>108</v>
-      </c>
-      <c r="B7" s="2" t="s">
+      <c r="E6" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="B7" t="s">
         <v>70</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="C7" t="s">
         <v>111</v>
       </c>
-      <c r="D7" s="2">
+      <c r="D7">
         <v>3350</v>
       </c>
-      <c r="E7" s="2" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="5" t="s">
-        <v>108</v>
-      </c>
-      <c r="B8" s="2" t="s">
+      <c r="E7" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="B8" t="s">
         <v>71</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="C8" t="s">
         <v>111</v>
       </c>
-      <c r="D8" s="2">
+      <c r="D8">
         <v>1150</v>
       </c>
-      <c r="E8" s="2" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="5" t="s">
-        <v>108</v>
-      </c>
-      <c r="B9" s="2" t="s">
+      <c r="E8" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="B9" t="s">
         <v>72</v>
       </c>
-      <c r="C9" s="3" t="s">
+      <c r="C9" t="s">
         <v>111</v>
       </c>
-      <c r="D9" s="2">
+      <c r="D9">
         <v>293</v>
       </c>
-      <c r="E9" s="2" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="5" t="s">
-        <v>108</v>
-      </c>
-      <c r="B10" s="2" t="s">
+      <c r="E9" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="B10" t="s">
         <v>73</v>
       </c>
-      <c r="C10" s="3" t="s">
+      <c r="C10" t="s">
         <v>111</v>
       </c>
-      <c r="D10" s="2">
+      <c r="D10">
         <v>591</v>
       </c>
-      <c r="E10" s="2" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="5" t="s">
-        <v>108</v>
-      </c>
-      <c r="B11" s="2" t="s">
+      <c r="E10" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="B11" t="s">
         <v>74</v>
       </c>
-      <c r="C11" s="3" t="s">
+      <c r="C11" t="s">
         <v>111</v>
       </c>
-      <c r="D11" s="2">
+      <c r="D11">
         <v>337</v>
       </c>
-      <c r="E11" s="2" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="5" t="s">
-        <v>108</v>
-      </c>
-      <c r="B12" s="2" t="s">
+      <c r="E11" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="B12" t="s">
         <v>75</v>
       </c>
-      <c r="C12" s="3" t="s">
+      <c r="C12" t="s">
         <v>111</v>
       </c>
-      <c r="D12" s="2">
+      <c r="D12">
         <v>53</v>
       </c>
-      <c r="E12" s="2" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="5" t="s">
-        <v>108</v>
-      </c>
-      <c r="B13" s="2" t="s">
+      <c r="E12" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="B13" t="s">
         <v>76</v>
       </c>
-      <c r="C13" s="3" t="s">
+      <c r="C13" t="s">
         <v>111</v>
       </c>
-      <c r="D13" s="2">
+      <c r="D13">
         <v>89</v>
       </c>
-      <c r="E13" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="I13" s="3"/>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="5" t="s">
-        <v>108</v>
-      </c>
-      <c r="B14" s="2" t="s">
+      <c r="E13" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="B14" t="s">
         <v>77</v>
       </c>
-      <c r="C14" s="3" t="s">
+      <c r="C14" t="s">
         <v>111</v>
       </c>
-      <c r="D14" s="2">
+      <c r="D14">
         <v>44</v>
       </c>
-      <c r="E14" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="I14" s="3"/>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" s="5" t="s">
-        <v>108</v>
-      </c>
-      <c r="B15" s="2" t="s">
+      <c r="E14" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="B15" t="s">
         <v>78</v>
       </c>
-      <c r="C15" s="3" t="s">
+      <c r="C15" t="s">
         <v>111</v>
       </c>
-      <c r="D15" s="2">
+      <c r="D15">
         <v>66</v>
       </c>
-      <c r="E15" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="I15" s="3"/>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" s="5" t="s">
-        <v>108</v>
-      </c>
-      <c r="B16" s="2" t="s">
+      <c r="E15" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="B16" t="s">
         <v>79</v>
       </c>
-      <c r="C16" s="3" t="s">
+      <c r="C16" t="s">
         <v>111</v>
       </c>
-      <c r="D16" s="2">
+      <c r="D16">
         <v>121</v>
       </c>
-      <c r="E16" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="I16" s="3"/>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A17" s="5" t="s">
-        <v>108</v>
-      </c>
-      <c r="B17" s="2" t="s">
+      <c r="E16" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="B17" t="s">
         <v>86</v>
       </c>
-      <c r="C17" s="3" t="s">
+      <c r="C17" t="s">
         <v>111</v>
       </c>
-      <c r="D17" s="2">
+      <c r="D17">
         <v>33</v>
       </c>
-      <c r="E17" s="2" t="s">
+      <c r="E17" t="s">
         <v>55</v>
       </c>
-      <c r="I17" s="3"/>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A18" s="5" t="s">
-        <v>108</v>
-      </c>
-      <c r="B18" s="2" t="s">
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="B18" t="s">
         <v>80</v>
       </c>
-      <c r="C18" s="3" t="s">
+      <c r="C18" t="s">
         <v>111</v>
       </c>
-      <c r="D18" s="2">
+      <c r="D18">
         <v>29</v>
       </c>
-      <c r="E18" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="I18" s="3"/>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A19" s="5" t="s">
-        <v>108</v>
-      </c>
-      <c r="B19" s="2" t="s">
+      <c r="E18" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="B19" t="s">
         <v>81</v>
       </c>
-      <c r="C19" s="3" t="s">
+      <c r="C19" t="s">
         <v>111</v>
       </c>
-      <c r="D19" s="2">
+      <c r="D19">
         <v>168</v>
       </c>
-      <c r="E19" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="I19" s="3"/>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A20" s="5" t="s">
-        <v>108</v>
-      </c>
-      <c r="B20" s="2" t="s">
+      <c r="E19" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="B20" t="s">
         <v>82</v>
       </c>
-      <c r="C20" s="3" t="s">
+      <c r="C20" t="s">
         <v>111</v>
       </c>
-      <c r="D20" s="2">
+      <c r="D20">
         <v>64</v>
       </c>
-      <c r="E20" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="I20" s="3"/>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A21" s="5" t="s">
-        <v>108</v>
-      </c>
-      <c r="B21" s="2" t="s">
+      <c r="E20" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="B21" t="s">
         <v>83</v>
       </c>
-      <c r="C21" s="3" t="s">
+      <c r="C21" t="s">
         <v>111</v>
       </c>
-      <c r="D21" s="2">
+      <c r="D21">
         <v>407</v>
       </c>
-      <c r="E21" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="I21" s="3"/>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A22" s="5" t="s">
-        <v>108</v>
-      </c>
-      <c r="B22" s="2" t="s">
+      <c r="E21" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="B22" t="s">
         <v>85</v>
       </c>
-      <c r="C22" s="3" t="s">
+      <c r="C22" t="s">
         <v>111</v>
       </c>
-      <c r="D22" s="2">
+      <c r="D22">
         <v>137</v>
       </c>
-      <c r="E22" s="2" t="s">
+      <c r="E22" t="s">
         <v>55</v>
       </c>
-      <c r="I22" s="3"/>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A23" s="5" t="s">
-        <v>108</v>
-      </c>
-      <c r="B23" s="2" t="s">
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="B23" t="s">
         <v>84</v>
       </c>
-      <c r="C23" s="3" t="s">
+      <c r="C23" t="s">
         <v>111</v>
       </c>
-      <c r="D23" s="2">
+      <c r="D23">
         <v>11</v>
       </c>
-      <c r="E23" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="I23" s="3"/>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A24" s="5" t="s">
-        <v>108</v>
-      </c>
-      <c r="B24" s="3" t="s">
+      <c r="E23" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="B24" t="s">
         <v>87</v>
       </c>
-      <c r="C24" s="3" t="s">
+      <c r="C24" t="s">
         <v>111</v>
       </c>
       <c r="D24">
@@ -2300,73 +2335,89 @@
       <c r="E24" t="s">
         <v>56</v>
       </c>
-      <c r="I24" s="3"/>
-    </row>
-    <row r="25" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="5" t="s">
-        <v>108</v>
-      </c>
-      <c r="B25" s="3" t="s">
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="B25" t="s">
         <v>114</v>
       </c>
-      <c r="C25" s="3" t="s">
+      <c r="C25" t="s">
         <v>111</v>
       </c>
-      <c r="D25" s="3">
+      <c r="D25">
         <v>120</v>
       </c>
-      <c r="E25" s="3" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="5" t="s">
-        <v>108</v>
-      </c>
-      <c r="B26" s="3" t="s">
+      <c r="E25" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="B26" t="s">
         <v>115</v>
       </c>
-      <c r="C26" s="3" t="s">
+      <c r="C26" t="s">
         <v>111</v>
       </c>
-      <c r="D26" s="3">
+      <c r="D26">
         <v>115</v>
       </c>
-      <c r="E26" s="3" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="5" t="s">
-        <v>108</v>
-      </c>
-      <c r="B27" s="3" t="s">
+      <c r="E26" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="B27" t="s">
         <v>116</v>
       </c>
-      <c r="C27" s="3" t="s">
+      <c r="C27" t="s">
         <v>111</v>
       </c>
-      <c r="D27" s="3">
+      <c r="D27">
         <v>98</v>
       </c>
-      <c r="E27" s="3" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A28" s="5" t="s">
-        <v>108</v>
-      </c>
-      <c r="B28" s="2" t="s">
+      <c r="E27" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="B28" t="s">
         <v>113</v>
       </c>
-      <c r="C28" s="3" t="s">
+      <c r="C28" t="s">
         <v>112</v>
       </c>
       <c r="D28">
         <v>1.264</v>
       </c>
       <c r="E28" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="B29" t="s">
+        <v>158</v>
+      </c>
+      <c r="C29" t="s">
+        <v>111</v>
+      </c>
+      <c r="D29">
+        <v>108</v>
+      </c>
+      <c r="E29" t="s">
         <v>56</v>
       </c>
     </row>
@@ -2377,22 +2428,22 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BBE77CEC-E9ED-4D7C-87C7-6AFD98461E9D}">
-  <dimension ref="A1:H27"/>
+  <dimension ref="A1:H28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C15" sqref="C15:C18"/>
+      <selection activeCell="H29" sqref="H29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="34.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="26.28515625" customWidth="1"/>
-    <col min="3" max="3" width="26.28515625" style="3" customWidth="1"/>
-    <col min="4" max="4" width="9.5703125" customWidth="1"/>
-    <col min="5" max="5" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.7109375" customWidth="1"/>
-    <col min="8" max="8" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="27.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="22.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
@@ -2402,7 +2453,7 @@
       <c r="B1" t="s">
         <v>40</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" t="s">
         <v>1</v>
       </c>
       <c r="D1" t="s">
@@ -2422,552 +2473,531 @@
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+      <c r="A2" t="s">
         <v>16</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" t="s">
         <v>65</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="E2" s="6" t="s">
+      <c r="D2" t="s">
+        <v>56</v>
+      </c>
+      <c r="E2" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="F2" s="6" t="s">
+      <c r="F2" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="G2" s="6" t="s">
+      <c r="G2" s="3" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
+      <c r="A3" t="s">
         <v>17</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" t="s">
         <v>66</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" t="s">
         <v>7</v>
       </c>
-      <c r="D3" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="E3" s="6" t="s">
+      <c r="D3" t="s">
+        <v>56</v>
+      </c>
+      <c r="E3" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="F3" s="6" t="s">
+      <c r="F3" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="G3" s="6" t="s">
+      <c r="G3" s="3" t="s">
         <v>130</v>
       </c>
-      <c r="H3" s="3"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
+      <c r="A4" t="s">
         <v>18</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" t="s">
         <v>67</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="E4" s="6" t="s">
+      <c r="D4" t="s">
+        <v>56</v>
+      </c>
+      <c r="E4" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="F4" s="6" t="s">
+      <c r="F4" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="G4" s="6" t="s">
+      <c r="G4" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="H4" s="3"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
+      <c r="A5" t="s">
         <v>19</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" t="s">
         <v>68</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="E5" s="6" t="s">
+      <c r="D5" t="s">
+        <v>56</v>
+      </c>
+      <c r="E5" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="F5" s="6" t="s">
+      <c r="F5" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="G5" s="6" t="s">
+      <c r="G5" s="3" t="s">
         <v>130</v>
       </c>
-      <c r="H5" s="3"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
+      <c r="A6" t="s">
         <v>20</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" t="s">
         <v>69</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C6" t="s">
         <v>10</v>
       </c>
-      <c r="D6" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="E6" s="6" t="s">
+      <c r="D6" t="s">
+        <v>56</v>
+      </c>
+      <c r="E6" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="F6" s="6" t="s">
+      <c r="F6" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="G6" s="6" t="s">
+      <c r="G6" s="3" t="s">
         <v>130</v>
       </c>
-      <c r="H6" s="3"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
+      <c r="A7" t="s">
         <v>21</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B7" t="s">
         <v>70</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="C7" t="s">
         <v>11</v>
       </c>
-      <c r="D7" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="E7" s="6" t="s">
+      <c r="D7" t="s">
+        <v>56</v>
+      </c>
+      <c r="E7" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="F7" s="6" t="s">
+      <c r="F7" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="G7" s="6" t="s">
+      <c r="G7" s="3" t="s">
         <v>130</v>
       </c>
-      <c r="H7" s="3"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
+      <c r="A8" t="s">
         <v>22</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B8" t="s">
         <v>71</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="C8" t="s">
         <v>12</v>
       </c>
-      <c r="D8" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="E8" s="6" t="s">
+      <c r="D8" t="s">
+        <v>56</v>
+      </c>
+      <c r="E8" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="F8" s="6" t="s">
+      <c r="F8" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="G8" s="6" t="s">
+      <c r="G8" s="3" t="s">
         <v>130</v>
       </c>
-      <c r="H8" s="3"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
+      <c r="A9" t="s">
         <v>23</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="B9" t="s">
         <v>72</v>
       </c>
-      <c r="C9" s="3" t="s">
+      <c r="C9" t="s">
         <v>13</v>
       </c>
-      <c r="D9" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="E9" s="6" t="s">
+      <c r="D9" t="s">
+        <v>56</v>
+      </c>
+      <c r="E9" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="F9" s="6" t="s">
+      <c r="F9" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="G9" s="6" t="s">
+      <c r="G9" s="3" t="s">
         <v>130</v>
       </c>
-      <c r="H9" s="3"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
+      <c r="A10" t="s">
         <v>24</v>
       </c>
-      <c r="B10" s="3" t="s">
+      <c r="B10" t="s">
         <v>73</v>
       </c>
-      <c r="C10" s="3" t="s">
+      <c r="C10" t="s">
         <v>14</v>
       </c>
-      <c r="D10" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="E10" s="6" t="s">
+      <c r="D10" t="s">
+        <v>56</v>
+      </c>
+      <c r="E10" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="F10" s="6" t="s">
+      <c r="F10" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="G10" s="6" t="s">
+      <c r="G10" s="3" t="s">
         <v>130</v>
       </c>
-      <c r="H10" s="3"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
+      <c r="A11" t="s">
         <v>25</v>
       </c>
-      <c r="B11" s="3" t="s">
+      <c r="B11" t="s">
         <v>74</v>
       </c>
-      <c r="C11" s="3" t="s">
+      <c r="C11" t="s">
         <v>15</v>
       </c>
-      <c r="D11" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="E11" s="6" t="s">
+      <c r="D11" t="s">
+        <v>56</v>
+      </c>
+      <c r="E11" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="F11" s="6" t="s">
+      <c r="F11" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="G11" s="6" t="s">
+      <c r="G11" s="3" t="s">
         <v>130</v>
       </c>
-      <c r="H11" s="3"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="2" t="s">
+      <c r="A12" t="s">
         <v>42</v>
       </c>
-      <c r="B12" s="3" t="s">
+      <c r="B12" t="s">
         <v>75</v>
       </c>
-      <c r="C12" s="3" t="s">
+      <c r="C12" t="s">
         <v>137</v>
       </c>
-      <c r="D12" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="E12" s="6" t="s">
+      <c r="D12" t="s">
+        <v>56</v>
+      </c>
+      <c r="E12" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="F12" s="6" t="s">
+      <c r="F12" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="G12" s="6" t="s">
+      <c r="G12" s="3" t="s">
         <v>130</v>
       </c>
-      <c r="H12" s="3"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="2" t="s">
+      <c r="A13" t="s">
         <v>43</v>
       </c>
-      <c r="B13" s="3" t="s">
+      <c r="B13" t="s">
         <v>76</v>
       </c>
-      <c r="C13" s="3" t="s">
+      <c r="C13" t="s">
         <v>138</v>
       </c>
-      <c r="D13" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="E13" s="6" t="s">
+      <c r="D13" t="s">
+        <v>56</v>
+      </c>
+      <c r="E13" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="F13" s="6" t="s">
+      <c r="F13" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="G13" s="6" t="s">
+      <c r="G13" s="3" t="s">
         <v>130</v>
       </c>
-      <c r="H13" s="3"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="2" t="s">
+      <c r="A14" t="s">
         <v>44</v>
       </c>
-      <c r="B14" s="3" t="s">
+      <c r="B14" t="s">
         <v>77</v>
       </c>
-      <c r="C14" s="3" t="s">
+      <c r="C14" t="s">
         <v>139</v>
       </c>
       <c r="D14" t="s">
         <v>56</v>
       </c>
-      <c r="E14" s="6" t="s">
+      <c r="E14" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="F14" s="6" t="s">
+      <c r="F14" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="G14" s="6" t="s">
+      <c r="G14" s="3" t="s">
         <v>130</v>
       </c>
-      <c r="H14" s="3"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>45</v>
       </c>
-      <c r="B15" s="3" t="s">
+      <c r="B15" t="s">
         <v>78</v>
       </c>
-      <c r="C15" s="3" t="s">
+      <c r="C15" t="s">
         <v>140</v>
       </c>
       <c r="D15" t="s">
         <v>56</v>
       </c>
-      <c r="E15" s="6" t="s">
+      <c r="E15" s="3" t="s">
         <v>121</v>
       </c>
-      <c r="F15" s="6" t="s">
+      <c r="F15" s="3" t="s">
         <v>122</v>
       </c>
-      <c r="G15" s="6" t="s">
+      <c r="G15" s="3" t="s">
         <v>130</v>
       </c>
-      <c r="H15" s="3"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>46</v>
       </c>
-      <c r="B16" s="3" t="s">
+      <c r="B16" t="s">
         <v>79</v>
       </c>
-      <c r="C16" s="3" t="s">
+      <c r="C16" t="s">
         <v>141</v>
       </c>
       <c r="D16" t="s">
         <v>56</v>
       </c>
-      <c r="E16" s="6" t="s">
+      <c r="E16" s="3" t="s">
         <v>121</v>
       </c>
-      <c r="F16" s="6" t="s">
+      <c r="F16" s="3" t="s">
         <v>122</v>
       </c>
-      <c r="G16" s="6" t="s">
+      <c r="G16" s="3" t="s">
         <v>130</v>
       </c>
-      <c r="H16" s="3"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>47</v>
       </c>
-      <c r="B17" s="3" t="s">
+      <c r="B17" t="s">
         <v>86</v>
       </c>
-      <c r="C17" s="3" t="s">
+      <c r="C17" t="s">
         <v>148</v>
       </c>
       <c r="D17" t="s">
         <v>55</v>
       </c>
-      <c r="E17" s="6" t="s">
+      <c r="E17" s="3" t="s">
         <v>121</v>
       </c>
-      <c r="F17" s="6" t="s">
+      <c r="F17" s="3" t="s">
         <v>122</v>
       </c>
-      <c r="G17" s="6" t="s">
+      <c r="G17" s="3" t="s">
         <v>128</v>
       </c>
-      <c r="H17" s="3"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>48</v>
       </c>
-      <c r="B18" s="3" t="s">
+      <c r="B18" t="s">
         <v>80</v>
       </c>
-      <c r="C18" s="3" t="s">
+      <c r="C18" t="s">
         <v>142</v>
       </c>
       <c r="D18" t="s">
         <v>56</v>
       </c>
-      <c r="E18" s="6" t="s">
+      <c r="E18" s="3" t="s">
         <v>121</v>
       </c>
-      <c r="F18" s="6" t="s">
+      <c r="F18" s="3" t="s">
         <v>122</v>
       </c>
-      <c r="G18" s="6" t="s">
+      <c r="G18" s="3" t="s">
         <v>129</v>
       </c>
-      <c r="H18" s="3"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>49</v>
       </c>
-      <c r="B19" s="3" t="s">
+      <c r="B19" t="s">
         <v>81</v>
       </c>
-      <c r="C19" s="3" t="s">
+      <c r="C19" t="s">
         <v>143</v>
       </c>
       <c r="D19" t="s">
         <v>56</v>
       </c>
-      <c r="E19" s="6" t="s">
+      <c r="E19" s="3" t="s">
         <v>123</v>
       </c>
-      <c r="F19" s="6" t="s">
+      <c r="F19" s="3" t="s">
         <v>124</v>
       </c>
-      <c r="G19" s="6" t="s">
+      <c r="G19" s="3" t="s">
         <v>130</v>
       </c>
-      <c r="H19" s="3"/>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>50</v>
       </c>
-      <c r="B20" s="3" t="s">
+      <c r="B20" t="s">
         <v>82</v>
       </c>
-      <c r="C20" s="3" t="s">
+      <c r="C20" t="s">
         <v>144</v>
       </c>
       <c r="D20" t="s">
         <v>56</v>
       </c>
-      <c r="E20" s="6" t="s">
+      <c r="E20" s="3" t="s">
         <v>123</v>
       </c>
-      <c r="F20" s="6" t="s">
+      <c r="F20" s="3" t="s">
         <v>124</v>
       </c>
-      <c r="G20" s="6" t="s">
+      <c r="G20" s="3" t="s">
         <v>130</v>
       </c>
-      <c r="H20" s="3"/>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>51</v>
       </c>
-      <c r="B21" s="3" t="s">
+      <c r="B21" t="s">
         <v>83</v>
       </c>
-      <c r="C21" s="3" t="s">
+      <c r="C21" t="s">
         <v>145</v>
       </c>
       <c r="D21" t="s">
         <v>56</v>
       </c>
-      <c r="E21" s="6" t="s">
+      <c r="E21" s="3" t="s">
         <v>123</v>
       </c>
-      <c r="F21" s="6" t="s">
+      <c r="F21" s="3" t="s">
         <v>124</v>
       </c>
-      <c r="G21" s="6" t="s">
+      <c r="G21" s="3" t="s">
         <v>130</v>
       </c>
-      <c r="H21" s="3"/>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>52</v>
       </c>
-      <c r="B22" s="3" t="s">
+      <c r="B22" t="s">
         <v>85</v>
       </c>
-      <c r="C22" s="3" t="s">
+      <c r="C22" t="s">
         <v>149</v>
       </c>
       <c r="D22" t="s">
         <v>55</v>
       </c>
-      <c r="E22" s="6" t="s">
+      <c r="E22" s="3" t="s">
         <v>123</v>
       </c>
-      <c r="F22" s="6" t="s">
+      <c r="F22" s="3" t="s">
         <v>124</v>
       </c>
-      <c r="G22" s="6" t="s">
+      <c r="G22" s="3" t="s">
         <v>128</v>
       </c>
-      <c r="H22" s="3"/>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>53</v>
       </c>
-      <c r="B23" s="3" t="s">
+      <c r="B23" t="s">
         <v>84</v>
       </c>
-      <c r="C23" s="3" t="s">
+      <c r="C23" t="s">
         <v>146</v>
       </c>
       <c r="D23" t="s">
         <v>56</v>
       </c>
-      <c r="E23" s="6" t="s">
+      <c r="E23" s="3" t="s">
         <v>123</v>
       </c>
-      <c r="F23" s="6" t="s">
+      <c r="F23" s="3" t="s">
         <v>124</v>
       </c>
-      <c r="G23" s="6" t="s">
+      <c r="G23" s="3" t="s">
         <v>129</v>
       </c>
-      <c r="H23" s="3"/>
-    </row>
-    <row r="24" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="3" t="s">
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
         <v>125</v>
       </c>
-      <c r="B24" s="3" t="s">
+      <c r="B24" t="s">
         <v>126</v>
       </c>
-      <c r="C24" s="3" t="s">
+      <c r="C24" t="s">
         <v>147</v>
       </c>
-      <c r="D24" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="E24" s="6" t="s">
+      <c r="D24" t="s">
+        <v>56</v>
+      </c>
+      <c r="E24" s="3" t="s">
         <v>123</v>
       </c>
-      <c r="F24" s="6" t="s">
+      <c r="F24" s="3" t="s">
         <v>127</v>
       </c>
-      <c r="G24" s="6" t="s">
+      <c r="G24" s="3" t="s">
         <v>130</v>
       </c>
     </row>
@@ -2978,19 +3008,19 @@
       <c r="B25" t="s">
         <v>115</v>
       </c>
-      <c r="D25" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="E25" s="6" t="s">
+      <c r="D25" t="s">
+        <v>56</v>
+      </c>
+      <c r="E25" s="3" t="s">
         <v>121</v>
       </c>
-      <c r="F25" s="6" t="s">
+      <c r="F25" s="3" t="s">
         <v>131</v>
       </c>
-      <c r="G25" s="6" t="s">
+      <c r="G25" s="3" t="s">
         <v>132</v>
       </c>
-      <c r="H25" s="3" t="s">
+      <c r="H25" t="s">
         <v>62</v>
       </c>
     </row>
@@ -3001,19 +3031,19 @@
       <c r="B26" t="s">
         <v>116</v>
       </c>
-      <c r="D26" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="E26" s="6" t="s">
+      <c r="D26" t="s">
+        <v>56</v>
+      </c>
+      <c r="E26" s="3" t="s">
         <v>123</v>
       </c>
-      <c r="F26" s="6" t="s">
+      <c r="F26" s="3" t="s">
         <v>131</v>
       </c>
-      <c r="G26" s="6" t="s">
+      <c r="G26" s="3" t="s">
         <v>132</v>
       </c>
-      <c r="H26" s="3" t="s">
+      <c r="H26" t="s">
         <v>63</v>
       </c>
     </row>
@@ -3024,20 +3054,43 @@
       <c r="B27" t="s">
         <v>114</v>
       </c>
-      <c r="D27" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="E27" s="6" t="s">
+      <c r="D27" t="s">
+        <v>56</v>
+      </c>
+      <c r="E27" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="F27" s="6" t="s">
+      <c r="F27" s="3" t="s">
         <v>131</v>
       </c>
-      <c r="G27" s="6" t="s">
+      <c r="G27" s="3" t="s">
         <v>130</v>
       </c>
-      <c r="H27" s="3" t="s">
+      <c r="H27" t="s">
         <v>64</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>157</v>
+      </c>
+      <c r="B28" t="s">
+        <v>158</v>
+      </c>
+      <c r="D28" t="s">
+        <v>56</v>
+      </c>
+      <c r="E28" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="F28" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="G28" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="H28" t="s">
+        <v>159</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Change to create 2 layers of ref portfolio (#529)
* Change to create 2 layers of ref portfolio

* Update Look-through valuation (multi-level).ipynb

* Update Look-through valuation (multi-level).ipynb
</commit_message>
<xml_diff>
--- a/examples/use-cases/valuation/data/lookthrough_data.xlsx
+++ b/examples/use-cases/valuation/data/lookthrough_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ThomasPartridge\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AndrewPoulter\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{065B1F0A-A63E-48F1-B2EF-147DCEF9317B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBE33215-F025-4C51-8363-D3E1CEAE9E90}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="12852" windowWidth="23256" windowHeight="14016" xr2:uid="{140D0F4F-AA5F-4E16-95A8-8F9F58C5F424}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{140D0F4F-AA5F-4E16-95A8-8F9F58C5F424}"/>
   </bookViews>
   <sheets>
     <sheet name="transactions" sheetId="3" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="520" uniqueCount="156">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="540" uniqueCount="160">
   <si>
     <t>date</t>
   </si>
@@ -505,6 +505,18 @@
   </si>
   <si>
     <t>cash_id</t>
+  </si>
+  <si>
+    <t>txnid_0021</t>
+  </si>
+  <si>
+    <t>USEquityFinancials Fund</t>
+  </si>
+  <si>
+    <t>fund_USEquityFinancials</t>
+  </si>
+  <si>
+    <t>USEquityFinancials</t>
   </si>
 </sst>
 </file>
@@ -557,12 +569,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -888,22 +895,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33E4483A-D81C-486B-9469-6BB1913F7014}">
-  <dimension ref="A1:L21"/>
+  <dimension ref="A1:L22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L23" sqref="L23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.85546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="19.85546875" style="3" customWidth="1"/>
-    <col min="6" max="6" width="22.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="19.85546875" customWidth="1"/>
+    <col min="6" max="6" width="26.7109375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="13.28515625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="28.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="18.42578125" style="3" customWidth="1"/>
+    <col min="9" max="9" width="18.42578125" customWidth="1"/>
     <col min="10" max="10" width="8.5703125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="12" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="18.5703125" bestFit="1" customWidth="1"/>
@@ -911,741 +918,780 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+      <c r="A1" t="s">
         <v>90</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="F1" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="G1" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="H1" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="I1" s="1" t="s">
         <v>155</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="J1" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="K1" s="4" t="s">
+      <c r="K1" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="L1" s="4" t="s">
+      <c r="L1" s="1" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+      <c r="A2" t="s">
         <v>93</v>
       </c>
-      <c r="B2" s="5" t="s">
-        <v>107</v>
-      </c>
-      <c r="C2" s="5" t="s">
+      <c r="B2" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="D2" s="5" t="s">
-        <v>107</v>
-      </c>
-      <c r="E2" s="5" t="s">
-        <v>108</v>
-      </c>
-      <c r="F2" s="3" t="s">
+      <c r="D2" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="F2" t="s">
         <v>64</v>
       </c>
-      <c r="G2" s="4">
+      <c r="G2" s="1">
         <v>2000</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="H2" t="s">
         <v>75</v>
       </c>
-      <c r="J2" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="K2" s="3">
+      <c r="J2" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="K2">
         <v>145.9</v>
       </c>
-      <c r="L2" s="3">
+      <c r="L2">
         <v>291800</v>
       </c>
     </row>
-    <row r="3" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>94</v>
       </c>
-      <c r="B3" s="5" t="s">
-        <v>107</v>
-      </c>
-      <c r="C3" s="5" t="s">
+      <c r="B3" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="D3" s="5" t="s">
-        <v>107</v>
-      </c>
-      <c r="E3" s="5" t="s">
-        <v>108</v>
-      </c>
-      <c r="F3" s="3" t="s">
+      <c r="D3" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="F3" t="s">
         <v>64</v>
       </c>
-      <c r="G3" s="4">
+      <c r="G3" s="1">
         <v>500</v>
       </c>
-      <c r="H3" s="3" t="s">
+      <c r="H3" t="s">
         <v>76</v>
       </c>
-      <c r="J3" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="K3" s="3">
+      <c r="J3" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="K3">
         <v>179.63</v>
       </c>
-      <c r="L3" s="3">
+      <c r="L3">
         <v>89815</v>
       </c>
     </row>
-    <row r="4" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>95</v>
       </c>
-      <c r="B4" s="5" t="s">
-        <v>107</v>
-      </c>
-      <c r="C4" s="5" t="s">
+      <c r="B4" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="D4" s="5" t="s">
-        <v>107</v>
-      </c>
-      <c r="E4" s="5" t="s">
-        <v>108</v>
-      </c>
-      <c r="F4" s="3" t="s">
+      <c r="D4" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="F4" t="s">
         <v>64</v>
       </c>
-      <c r="G4" s="4">
+      <c r="G4" s="1">
         <v>750</v>
       </c>
-      <c r="H4" s="3" t="s">
+      <c r="H4" t="s">
         <v>77</v>
       </c>
-      <c r="J4" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="K4" s="3">
+      <c r="J4" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="K4">
         <v>120.05</v>
       </c>
-      <c r="L4" s="3">
+      <c r="L4">
         <v>90037.5</v>
       </c>
     </row>
-    <row r="5" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>96</v>
       </c>
-      <c r="B5" s="5" t="s">
-        <v>107</v>
-      </c>
-      <c r="C5" s="5" t="s">
+      <c r="B5" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="C5" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="D5" s="5" t="s">
-        <v>107</v>
-      </c>
-      <c r="E5" s="5" t="s">
-        <v>108</v>
-      </c>
-      <c r="F5" s="3" t="s">
+      <c r="D5" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="F5" t="s">
         <v>64</v>
       </c>
-      <c r="G5" s="4">
+      <c r="G5" s="1">
         <v>100</v>
       </c>
-      <c r="H5" s="3" t="s">
+      <c r="H5" t="s">
         <v>87</v>
       </c>
-      <c r="J5" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="K5" s="3">
+      <c r="J5" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="K5">
         <v>7469.99</v>
       </c>
-      <c r="L5" s="3">
+      <c r="L5">
         <v>746999</v>
       </c>
     </row>
-    <row r="6" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>97</v>
       </c>
-      <c r="B6" s="5" t="s">
-        <v>107</v>
-      </c>
-      <c r="C6" s="5" t="s">
+      <c r="B6" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="C6" s="2" t="s">
         <v>154</v>
       </c>
-      <c r="D6" s="5" t="s">
-        <v>107</v>
-      </c>
-      <c r="E6" s="5" t="s">
-        <v>108</v>
-      </c>
-      <c r="F6" s="3" t="s">
+      <c r="D6" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="F6" t="s">
         <v>64</v>
       </c>
-      <c r="G6" s="4">
+      <c r="G6" s="1">
         <v>1300000</v>
       </c>
-      <c r="I6" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="J6" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="K6" s="3">
+      <c r="I6" t="s">
+        <v>56</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="K6">
         <v>1</v>
       </c>
-      <c r="L6" s="3">
+      <c r="L6">
         <v>1300000</v>
       </c>
     </row>
-    <row r="7" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>98</v>
       </c>
-      <c r="B7" s="5" t="s">
-        <v>107</v>
-      </c>
-      <c r="C7" s="5" t="s">
+      <c r="B7" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="C7" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="D7" s="5" t="s">
-        <v>107</v>
-      </c>
-      <c r="E7" s="5" t="s">
-        <v>108</v>
-      </c>
-      <c r="F7" s="3" t="s">
+      <c r="D7" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="F7" t="s">
         <v>62</v>
       </c>
-      <c r="G7" s="4">
+      <c r="G7" s="1">
         <v>5000</v>
       </c>
-      <c r="H7" s="3" t="s">
+      <c r="H7" t="s">
         <v>80</v>
       </c>
-      <c r="J7" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="K7" s="3">
+      <c r="J7" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="K7">
         <v>29.01</v>
       </c>
-      <c r="L7" s="3">
+      <c r="L7">
         <v>145050</v>
       </c>
     </row>
-    <row r="8" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>99</v>
       </c>
-      <c r="B8" s="5" t="s">
-        <v>107</v>
-      </c>
-      <c r="C8" s="5" t="s">
+      <c r="B8" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="C8" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="D8" s="5" t="s">
-        <v>107</v>
-      </c>
-      <c r="E8" s="5" t="s">
-        <v>108</v>
-      </c>
-      <c r="F8" s="3" t="s">
+      <c r="D8" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="F8" t="s">
         <v>62</v>
       </c>
-      <c r="G8" s="4">
+      <c r="G8" s="1">
         <v>750</v>
       </c>
-      <c r="H8" s="3" t="s">
+      <c r="H8" t="s">
         <v>78</v>
       </c>
-      <c r="J8" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="K8" s="3">
+      <c r="J8" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="K8">
         <v>65.819999999999993</v>
       </c>
-      <c r="L8" s="3">
+      <c r="L8">
         <v>49364.999999999993</v>
       </c>
     </row>
-    <row r="9" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="3" t="s">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
         <v>100</v>
       </c>
-      <c r="B9" s="5" t="s">
-        <v>107</v>
-      </c>
-      <c r="C9" s="5" t="s">
+      <c r="B9" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="C9" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="D9" s="5" t="s">
-        <v>107</v>
-      </c>
-      <c r="E9" s="5" t="s">
-        <v>108</v>
-      </c>
-      <c r="F9" s="3" t="s">
+      <c r="D9" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="F9" t="s">
         <v>62</v>
       </c>
-      <c r="G9" s="4">
+      <c r="G9" s="1">
         <v>3000</v>
       </c>
-      <c r="H9" s="3" t="s">
+      <c r="H9" t="s">
         <v>79</v>
       </c>
-      <c r="J9" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="K9" s="3">
+      <c r="J9" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="K9">
         <v>121.16</v>
       </c>
-      <c r="L9" s="3">
+      <c r="L9">
         <v>363480</v>
       </c>
     </row>
-    <row r="10" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="3" t="s">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
         <v>101</v>
       </c>
-      <c r="B10" s="5" t="s">
-        <v>107</v>
-      </c>
-      <c r="C10" s="5" t="s">
+      <c r="B10" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="C10" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="D10" s="5" t="s">
-        <v>107</v>
-      </c>
-      <c r="E10" s="5" t="s">
-        <v>108</v>
-      </c>
-      <c r="F10" s="3" t="s">
+      <c r="D10" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="F10" t="s">
         <v>62</v>
       </c>
-      <c r="G10" s="4">
+      <c r="G10" s="1">
         <v>1000</v>
       </c>
-      <c r="H10" s="3" t="s">
+      <c r="H10" t="s">
         <v>86</v>
       </c>
-      <c r="J10" s="4" t="s">
+      <c r="J10" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="K10" s="3">
+      <c r="K10">
         <v>32.840000000000003</v>
       </c>
-      <c r="L10" s="3">
+      <c r="L10">
         <v>32840</v>
       </c>
     </row>
-    <row r="11" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="3" t="s">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
         <v>102</v>
       </c>
-      <c r="B11" s="5" t="s">
-        <v>107</v>
-      </c>
-      <c r="C11" s="5" t="s">
+      <c r="B11" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="C11" s="2" t="s">
         <v>154</v>
       </c>
-      <c r="D11" s="5" t="s">
-        <v>107</v>
-      </c>
-      <c r="E11" s="5" t="s">
-        <v>108</v>
-      </c>
-      <c r="F11" s="3" t="s">
+      <c r="D11" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="F11" t="s">
         <v>62</v>
       </c>
-      <c r="G11" s="4">
+      <c r="G11" s="1">
         <v>700000</v>
       </c>
-      <c r="I11" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="J11" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="K11" s="3">
+      <c r="I11" t="s">
+        <v>56</v>
+      </c>
+      <c r="J11" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="K11">
         <v>1</v>
       </c>
-      <c r="L11" s="3">
+      <c r="L11">
         <v>700000</v>
       </c>
     </row>
-    <row r="12" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="3" t="s">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
         <v>103</v>
       </c>
-      <c r="B12" s="5" t="s">
-        <v>107</v>
-      </c>
-      <c r="C12" s="5" t="s">
+      <c r="B12" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="C12" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="D12" s="5" t="s">
-        <v>107</v>
-      </c>
-      <c r="E12" s="5" t="s">
-        <v>108</v>
-      </c>
-      <c r="F12" s="3" t="s">
+      <c r="D12" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="F12" t="s">
+        <v>159</v>
+      </c>
+      <c r="G12" s="1">
+        <v>250</v>
+      </c>
+      <c r="H12" t="s">
+        <v>81</v>
+      </c>
+      <c r="J12" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="K12">
+        <v>167.87</v>
+      </c>
+      <c r="L12">
+        <v>41967.5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>104</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="F13" t="s">
+        <v>159</v>
+      </c>
+      <c r="G13" s="1">
+        <v>1000</v>
+      </c>
+      <c r="H13" t="s">
+        <v>82</v>
+      </c>
+      <c r="J13" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="K13">
+        <v>64.25</v>
+      </c>
+      <c r="L13">
+        <v>64250</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>105</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="F14" t="s">
+        <v>159</v>
+      </c>
+      <c r="G14" s="1">
+        <v>100</v>
+      </c>
+      <c r="H14" t="s">
+        <v>83</v>
+      </c>
+      <c r="J14" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="K14">
+        <v>407.33</v>
+      </c>
+      <c r="L14">
+        <v>40733</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>118</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="F15" t="s">
         <v>63</v>
       </c>
-      <c r="G12" s="4">
-        <v>250</v>
-      </c>
-      <c r="H12" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="J12" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="K12" s="3">
-        <v>167.87</v>
-      </c>
-      <c r="L12" s="3">
-        <v>41967.5</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="3" t="s">
-        <v>104</v>
-      </c>
-      <c r="B13" s="5" t="s">
-        <v>107</v>
-      </c>
-      <c r="C13" s="5" t="s">
+      <c r="G15" s="1">
+        <v>5000</v>
+      </c>
+      <c r="H15" t="s">
+        <v>85</v>
+      </c>
+      <c r="J15" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="K15">
+        <v>137.22</v>
+      </c>
+      <c r="L15">
+        <v>686100</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>119</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="C16" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="D13" s="5" t="s">
-        <v>107</v>
-      </c>
-      <c r="E13" s="5" t="s">
-        <v>108</v>
-      </c>
-      <c r="F13" s="3" t="s">
+      <c r="D16" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="F16" t="s">
         <v>63</v>
       </c>
-      <c r="G13" s="4">
-        <v>1000</v>
-      </c>
-      <c r="H13" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="J13" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="K13" s="3">
-        <v>64.25</v>
-      </c>
-      <c r="L13" s="3">
-        <v>64250</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="3" t="s">
-        <v>105</v>
-      </c>
-      <c r="B14" s="5" t="s">
-        <v>107</v>
-      </c>
-      <c r="C14" s="5" t="s">
+      <c r="G16" s="1">
+        <v>350</v>
+      </c>
+      <c r="H16" t="s">
+        <v>84</v>
+      </c>
+      <c r="J16" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="K16">
+        <v>11.3</v>
+      </c>
+      <c r="L16">
+        <v>3955.0000000000005</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>120</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="F17" t="s">
+        <v>63</v>
+      </c>
+      <c r="G17" s="1">
+        <v>1000000</v>
+      </c>
+      <c r="I17" t="s">
+        <v>56</v>
+      </c>
+      <c r="J17" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="K17">
+        <v>1</v>
+      </c>
+      <c r="L17">
+        <v>1000000</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>150</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="C18" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="D14" s="5" t="s">
-        <v>107</v>
-      </c>
-      <c r="E14" s="5" t="s">
-        <v>108</v>
-      </c>
-      <c r="F14" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="G14" s="4">
-        <v>100</v>
-      </c>
-      <c r="H14" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="J14" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="K14" s="3">
-        <v>407.33</v>
-      </c>
-      <c r="L14" s="3">
-        <v>40733</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="3" t="s">
-        <v>118</v>
-      </c>
-      <c r="B15" s="5" t="s">
-        <v>107</v>
-      </c>
-      <c r="C15" s="5" t="s">
-        <v>92</v>
-      </c>
-      <c r="D15" s="5" t="s">
-        <v>107</v>
-      </c>
-      <c r="E15" s="5" t="s">
-        <v>108</v>
-      </c>
-      <c r="F15" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="G15" s="4">
-        <v>5000</v>
-      </c>
-      <c r="H15" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="J15" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="K15" s="3">
-        <v>137.22</v>
-      </c>
-      <c r="L15" s="3">
-        <v>686100</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="3" t="s">
-        <v>119</v>
-      </c>
-      <c r="B16" s="5" t="s">
-        <v>107</v>
-      </c>
-      <c r="C16" s="5" t="s">
-        <v>92</v>
-      </c>
-      <c r="D16" s="5" t="s">
-        <v>107</v>
-      </c>
-      <c r="E16" s="5" t="s">
-        <v>108</v>
-      </c>
-      <c r="F16" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="G16" s="4">
-        <v>350</v>
-      </c>
-      <c r="H16" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="J16" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="K16" s="3">
-        <v>11.3</v>
-      </c>
-      <c r="L16" s="3">
-        <v>3955.0000000000005</v>
-      </c>
-    </row>
-    <row r="17" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="3" t="s">
-        <v>120</v>
-      </c>
-      <c r="B17" s="5" t="s">
-        <v>107</v>
-      </c>
-      <c r="C17" s="5" t="s">
-        <v>154</v>
-      </c>
-      <c r="D17" s="5" t="s">
-        <v>107</v>
-      </c>
-      <c r="E17" s="5" t="s">
-        <v>108</v>
-      </c>
-      <c r="F17" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="G17" s="4">
-        <v>1000000</v>
-      </c>
-      <c r="I17" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="J17" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="K17" s="3">
-        <v>1</v>
-      </c>
-      <c r="L17" s="3">
-        <v>1000000</v>
-      </c>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A18" s="3" t="s">
-        <v>150</v>
-      </c>
-      <c r="B18" s="5" t="s">
-        <v>107</v>
-      </c>
-      <c r="C18" s="5" t="s">
-        <v>92</v>
-      </c>
-      <c r="D18" s="5" t="s">
-        <v>107</v>
-      </c>
-      <c r="E18" s="5" t="s">
-        <v>108</v>
-      </c>
-      <c r="F18" s="3" t="s">
+      <c r="D18" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="F18" t="s">
         <v>117</v>
       </c>
-      <c r="G18" s="4">
+      <c r="G18" s="1">
         <v>50</v>
       </c>
-      <c r="H18" s="3" t="s">
+      <c r="H18" t="s">
         <v>114</v>
       </c>
-      <c r="J18" s="4" t="s">
+      <c r="J18" s="1" t="s">
         <v>56</v>
       </c>
       <c r="K18">
         <v>119.5</v>
       </c>
-      <c r="L18" s="3">
+      <c r="L18">
         <v>5975</v>
       </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A19" s="3" t="s">
+      <c r="A19" t="s">
         <v>151</v>
       </c>
-      <c r="B19" s="5" t="s">
-        <v>107</v>
-      </c>
-      <c r="C19" s="5" t="s">
+      <c r="B19" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="C19" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="D19" s="5" t="s">
-        <v>107</v>
-      </c>
-      <c r="E19" s="5" t="s">
-        <v>108</v>
-      </c>
-      <c r="F19" s="3" t="s">
+      <c r="D19" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="F19" t="s">
         <v>117</v>
       </c>
-      <c r="G19" s="4">
+      <c r="G19" s="1">
         <v>50</v>
       </c>
-      <c r="H19" s="3" t="s">
+      <c r="H19" t="s">
         <v>115</v>
       </c>
-      <c r="J19" s="4" t="s">
+      <c r="J19" s="1" t="s">
         <v>56</v>
       </c>
       <c r="K19">
         <v>114</v>
       </c>
-      <c r="L19" s="3">
+      <c r="L19">
         <v>5700</v>
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A20" s="3" t="s">
+      <c r="A20" t="s">
         <v>152</v>
       </c>
-      <c r="B20" s="5" t="s">
-        <v>107</v>
-      </c>
-      <c r="C20" s="5" t="s">
+      <c r="B20" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="C20" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="D20" s="5" t="s">
-        <v>107</v>
-      </c>
-      <c r="E20" s="5" t="s">
-        <v>108</v>
-      </c>
-      <c r="F20" s="3" t="s">
+      <c r="D20" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="F20" t="s">
         <v>117</v>
       </c>
-      <c r="G20" s="4">
+      <c r="G20" s="1">
         <v>50</v>
       </c>
-      <c r="H20" s="3" t="s">
+      <c r="H20" t="s">
         <v>116</v>
       </c>
-      <c r="J20" s="4" t="s">
+      <c r="J20" s="1" t="s">
         <v>56</v>
       </c>
       <c r="K20">
         <v>96</v>
       </c>
-      <c r="L20" s="3">
+      <c r="L20">
         <v>4800</v>
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A21" s="3" t="s">
+      <c r="A21" t="s">
         <v>153</v>
       </c>
-      <c r="B21" s="5" t="s">
-        <v>107</v>
-      </c>
-      <c r="C21" s="5" t="s">
+      <c r="B21" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="C21" s="2" t="s">
         <v>154</v>
       </c>
-      <c r="D21" s="5" t="s">
-        <v>107</v>
-      </c>
-      <c r="E21" s="5" t="s">
-        <v>108</v>
-      </c>
-      <c r="F21" s="3" t="s">
+      <c r="D21" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="F21" t="s">
         <v>117</v>
       </c>
-      <c r="G21" s="4">
+      <c r="G21" s="1">
         <v>20000</v>
       </c>
-      <c r="I21" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="J21" s="4" t="s">
+      <c r="I21" t="s">
+        <v>56</v>
+      </c>
+      <c r="J21" s="1" t="s">
         <v>56</v>
       </c>
       <c r="K21">
         <v>1</v>
       </c>
-      <c r="L21" s="3">
+      <c r="L21">
         <v>20000</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>156</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="F22" t="s">
+        <v>63</v>
+      </c>
+      <c r="G22" s="1">
+        <v>25</v>
+      </c>
+      <c r="H22" t="s">
+        <v>158</v>
+      </c>
+      <c r="I22" t="s">
+        <v>56</v>
+      </c>
+      <c r="J22" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="K22">
+        <v>106</v>
+      </c>
+      <c r="L22">
+        <f>K22*G22</f>
+        <v>2650</v>
       </c>
     </row>
   </sheetData>
@@ -1665,7 +1711,7 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="7.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="17.85546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="7.140625" bestFit="1" customWidth="1"/>
@@ -1675,7 +1721,7 @@
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" t="s">
         <v>54</v>
       </c>
       <c r="C1" t="s">
@@ -1689,10 +1735,10 @@
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="s">
-        <v>108</v>
-      </c>
-      <c r="B2" s="2" t="s">
+      <c r="A2" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="B2" t="s">
         <v>57</v>
       </c>
       <c r="C2" t="s">
@@ -1706,10 +1752,10 @@
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="5" t="s">
-        <v>108</v>
-      </c>
-      <c r="B3" s="2" t="s">
+      <c r="A3" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="B3" t="s">
         <v>57</v>
       </c>
       <c r="C3" t="s">
@@ -1718,15 +1764,15 @@
       <c r="D3" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="E3" s="4">
+      <c r="E3" s="1">
         <v>0.1</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="5" t="s">
-        <v>108</v>
-      </c>
-      <c r="B4" s="2" t="s">
+      <c r="A4" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="B4" t="s">
         <v>57</v>
       </c>
       <c r="C4" t="s">
@@ -1735,15 +1781,15 @@
       <c r="D4" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="E4" s="4">
+      <c r="E4" s="1">
         <v>0.1</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="5" t="s">
-        <v>108</v>
-      </c>
-      <c r="B5" s="2" t="s">
+      <c r="A5" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="B5" t="s">
         <v>57</v>
       </c>
       <c r="C5" t="s">
@@ -1752,15 +1798,15 @@
       <c r="D5" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="E5" s="4">
+      <c r="E5" s="1">
         <v>0.1</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="5" t="s">
-        <v>108</v>
-      </c>
-      <c r="B6" s="2" t="s">
+      <c r="A6" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="B6" t="s">
         <v>57</v>
       </c>
       <c r="C6" t="s">
@@ -1769,15 +1815,15 @@
       <c r="D6" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="E6" s="4">
+      <c r="E6" s="1">
         <v>0.1</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="5" t="s">
-        <v>108</v>
-      </c>
-      <c r="B7" s="2" t="s">
+      <c r="A7" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="B7" t="s">
         <v>57</v>
       </c>
       <c r="C7" t="s">
@@ -1786,15 +1832,15 @@
       <c r="D7" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="E7" s="4">
+      <c r="E7" s="1">
         <v>0.1</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="5" t="s">
-        <v>108</v>
-      </c>
-      <c r="B8" s="2" t="s">
+      <c r="A8" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="B8" t="s">
         <v>57</v>
       </c>
       <c r="C8" t="s">
@@ -1803,15 +1849,15 @@
       <c r="D8" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="E8" s="4">
+      <c r="E8" s="1">
         <v>0.1</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="5" t="s">
-        <v>108</v>
-      </c>
-      <c r="B9" s="2" t="s">
+      <c r="A9" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="B9" t="s">
         <v>57</v>
       </c>
       <c r="C9" t="s">
@@ -1820,15 +1866,15 @@
       <c r="D9" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="E9" s="4">
+      <c r="E9" s="1">
         <v>0.1</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="5" t="s">
-        <v>108</v>
-      </c>
-      <c r="B10" s="2" t="s">
+      <c r="A10" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="B10" t="s">
         <v>57</v>
       </c>
       <c r="C10" t="s">
@@ -1837,15 +1883,15 @@
       <c r="D10" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="E10" s="4">
+      <c r="E10" s="1">
         <v>0.1</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="5" t="s">
-        <v>108</v>
-      </c>
-      <c r="B11" s="2" t="s">
+      <c r="A11" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="B11" t="s">
         <v>57</v>
       </c>
       <c r="C11" t="s">
@@ -1854,7 +1900,7 @@
       <c r="D11" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="E11" s="4">
+      <c r="E11" s="1">
         <v>0.1</v>
       </c>
     </row>
@@ -1867,431 +1913,420 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E615609-E297-47FD-9AAE-07E524F332F5}">
-  <dimension ref="A1:I28"/>
+  <dimension ref="A1:E29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A29" sqref="A29"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="27.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="6" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="8.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" t="s">
         <v>109</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" t="s">
         <v>110</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" t="s">
         <v>41</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="s">
-        <v>108</v>
-      </c>
-      <c r="B2" s="2" t="s">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="B2" t="s">
         <v>65</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" t="s">
         <v>111</v>
       </c>
-      <c r="D2" s="2">
+      <c r="D2">
         <v>146</v>
       </c>
-      <c r="E2" s="2" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="5" t="s">
-        <v>108</v>
-      </c>
-      <c r="B3" s="2" t="s">
+      <c r="E2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="B3" t="s">
         <v>66</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" t="s">
         <v>111</v>
       </c>
-      <c r="D3" s="2">
+      <c r="D3">
         <v>180</v>
       </c>
-      <c r="E3" s="2" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="5" t="s">
-        <v>108</v>
-      </c>
-      <c r="B4" s="2" t="s">
+      <c r="E3" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="B4" t="s">
         <v>67</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" t="s">
         <v>111</v>
       </c>
-      <c r="D4" s="2">
+      <c r="D4">
         <v>120</v>
       </c>
-      <c r="E4" s="2" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="5" t="s">
-        <v>108</v>
-      </c>
-      <c r="B5" s="2" t="s">
+      <c r="E4" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="B5" t="s">
         <v>68</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" t="s">
         <v>111</v>
       </c>
-      <c r="D5" s="2">
+      <c r="D5">
         <v>2888</v>
       </c>
-      <c r="E5" s="2" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="5" t="s">
-        <v>108</v>
-      </c>
-      <c r="B6" s="2" t="s">
+      <c r="E5" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="B6" t="s">
         <v>69</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C6" t="s">
         <v>111</v>
       </c>
-      <c r="D6" s="2">
+      <c r="D6">
         <v>329</v>
       </c>
-      <c r="E6" s="2" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="5" t="s">
-        <v>108</v>
-      </c>
-      <c r="B7" s="2" t="s">
+      <c r="E6" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="B7" t="s">
         <v>70</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="C7" t="s">
         <v>111</v>
       </c>
-      <c r="D7" s="2">
+      <c r="D7">
         <v>3350</v>
       </c>
-      <c r="E7" s="2" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="5" t="s">
-        <v>108</v>
-      </c>
-      <c r="B8" s="2" t="s">
+      <c r="E7" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="B8" t="s">
         <v>71</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="C8" t="s">
         <v>111</v>
       </c>
-      <c r="D8" s="2">
+      <c r="D8">
         <v>1150</v>
       </c>
-      <c r="E8" s="2" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="5" t="s">
-        <v>108</v>
-      </c>
-      <c r="B9" s="2" t="s">
+      <c r="E8" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="B9" t="s">
         <v>72</v>
       </c>
-      <c r="C9" s="3" t="s">
+      <c r="C9" t="s">
         <v>111</v>
       </c>
-      <c r="D9" s="2">
+      <c r="D9">
         <v>293</v>
       </c>
-      <c r="E9" s="2" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="5" t="s">
-        <v>108</v>
-      </c>
-      <c r="B10" s="2" t="s">
+      <c r="E9" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="B10" t="s">
         <v>73</v>
       </c>
-      <c r="C10" s="3" t="s">
+      <c r="C10" t="s">
         <v>111</v>
       </c>
-      <c r="D10" s="2">
+      <c r="D10">
         <v>591</v>
       </c>
-      <c r="E10" s="2" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="5" t="s">
-        <v>108</v>
-      </c>
-      <c r="B11" s="2" t="s">
+      <c r="E10" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="B11" t="s">
         <v>74</v>
       </c>
-      <c r="C11" s="3" t="s">
+      <c r="C11" t="s">
         <v>111</v>
       </c>
-      <c r="D11" s="2">
+      <c r="D11">
         <v>337</v>
       </c>
-      <c r="E11" s="2" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="5" t="s">
-        <v>108</v>
-      </c>
-      <c r="B12" s="2" t="s">
+      <c r="E11" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="B12" t="s">
         <v>75</v>
       </c>
-      <c r="C12" s="3" t="s">
+      <c r="C12" t="s">
         <v>111</v>
       </c>
-      <c r="D12" s="2">
+      <c r="D12">
         <v>53</v>
       </c>
-      <c r="E12" s="2" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="5" t="s">
-        <v>108</v>
-      </c>
-      <c r="B13" s="2" t="s">
+      <c r="E12" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="B13" t="s">
         <v>76</v>
       </c>
-      <c r="C13" s="3" t="s">
+      <c r="C13" t="s">
         <v>111</v>
       </c>
-      <c r="D13" s="2">
+      <c r="D13">
         <v>89</v>
       </c>
-      <c r="E13" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="I13" s="3"/>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="5" t="s">
-        <v>108</v>
-      </c>
-      <c r="B14" s="2" t="s">
+      <c r="E13" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="B14" t="s">
         <v>77</v>
       </c>
-      <c r="C14" s="3" t="s">
+      <c r="C14" t="s">
         <v>111</v>
       </c>
-      <c r="D14" s="2">
+      <c r="D14">
         <v>44</v>
       </c>
-      <c r="E14" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="I14" s="3"/>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" s="5" t="s">
-        <v>108</v>
-      </c>
-      <c r="B15" s="2" t="s">
+      <c r="E14" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="B15" t="s">
         <v>78</v>
       </c>
-      <c r="C15" s="3" t="s">
+      <c r="C15" t="s">
         <v>111</v>
       </c>
-      <c r="D15" s="2">
+      <c r="D15">
         <v>66</v>
       </c>
-      <c r="E15" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="I15" s="3"/>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" s="5" t="s">
-        <v>108</v>
-      </c>
-      <c r="B16" s="2" t="s">
+      <c r="E15" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="B16" t="s">
         <v>79</v>
       </c>
-      <c r="C16" s="3" t="s">
+      <c r="C16" t="s">
         <v>111</v>
       </c>
-      <c r="D16" s="2">
+      <c r="D16">
         <v>121</v>
       </c>
-      <c r="E16" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="I16" s="3"/>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A17" s="5" t="s">
-        <v>108</v>
-      </c>
-      <c r="B17" s="2" t="s">
+      <c r="E16" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="B17" t="s">
         <v>86</v>
       </c>
-      <c r="C17" s="3" t="s">
+      <c r="C17" t="s">
         <v>111</v>
       </c>
-      <c r="D17" s="2">
+      <c r="D17">
         <v>33</v>
       </c>
-      <c r="E17" s="2" t="s">
+      <c r="E17" t="s">
         <v>55</v>
       </c>
-      <c r="I17" s="3"/>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A18" s="5" t="s">
-        <v>108</v>
-      </c>
-      <c r="B18" s="2" t="s">
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="B18" t="s">
         <v>80</v>
       </c>
-      <c r="C18" s="3" t="s">
+      <c r="C18" t="s">
         <v>111</v>
       </c>
-      <c r="D18" s="2">
+      <c r="D18">
         <v>29</v>
       </c>
-      <c r="E18" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="I18" s="3"/>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A19" s="5" t="s">
-        <v>108</v>
-      </c>
-      <c r="B19" s="2" t="s">
+      <c r="E18" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="B19" t="s">
         <v>81</v>
       </c>
-      <c r="C19" s="3" t="s">
+      <c r="C19" t="s">
         <v>111</v>
       </c>
-      <c r="D19" s="2">
+      <c r="D19">
         <v>168</v>
       </c>
-      <c r="E19" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="I19" s="3"/>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A20" s="5" t="s">
-        <v>108</v>
-      </c>
-      <c r="B20" s="2" t="s">
+      <c r="E19" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="B20" t="s">
         <v>82</v>
       </c>
-      <c r="C20" s="3" t="s">
+      <c r="C20" t="s">
         <v>111</v>
       </c>
-      <c r="D20" s="2">
+      <c r="D20">
         <v>64</v>
       </c>
-      <c r="E20" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="I20" s="3"/>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A21" s="5" t="s">
-        <v>108</v>
-      </c>
-      <c r="B21" s="2" t="s">
+      <c r="E20" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="B21" t="s">
         <v>83</v>
       </c>
-      <c r="C21" s="3" t="s">
+      <c r="C21" t="s">
         <v>111</v>
       </c>
-      <c r="D21" s="2">
+      <c r="D21">
         <v>407</v>
       </c>
-      <c r="E21" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="I21" s="3"/>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A22" s="5" t="s">
-        <v>108</v>
-      </c>
-      <c r="B22" s="2" t="s">
+      <c r="E21" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="B22" t="s">
         <v>85</v>
       </c>
-      <c r="C22" s="3" t="s">
+      <c r="C22" t="s">
         <v>111</v>
       </c>
-      <c r="D22" s="2">
+      <c r="D22">
         <v>137</v>
       </c>
-      <c r="E22" s="2" t="s">
+      <c r="E22" t="s">
         <v>55</v>
       </c>
-      <c r="I22" s="3"/>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A23" s="5" t="s">
-        <v>108</v>
-      </c>
-      <c r="B23" s="2" t="s">
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="B23" t="s">
         <v>84</v>
       </c>
-      <c r="C23" s="3" t="s">
+      <c r="C23" t="s">
         <v>111</v>
       </c>
-      <c r="D23" s="2">
+      <c r="D23">
         <v>11</v>
       </c>
-      <c r="E23" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="I23" s="3"/>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A24" s="5" t="s">
-        <v>108</v>
-      </c>
-      <c r="B24" s="3" t="s">
+      <c r="E23" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="B24" t="s">
         <v>87</v>
       </c>
-      <c r="C24" s="3" t="s">
+      <c r="C24" t="s">
         <v>111</v>
       </c>
       <c r="D24">
@@ -2300,73 +2335,89 @@
       <c r="E24" t="s">
         <v>56</v>
       </c>
-      <c r="I24" s="3"/>
-    </row>
-    <row r="25" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="5" t="s">
-        <v>108</v>
-      </c>
-      <c r="B25" s="3" t="s">
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="B25" t="s">
         <v>114</v>
       </c>
-      <c r="C25" s="3" t="s">
+      <c r="C25" t="s">
         <v>111</v>
       </c>
-      <c r="D25" s="3">
+      <c r="D25">
         <v>120</v>
       </c>
-      <c r="E25" s="3" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="5" t="s">
-        <v>108</v>
-      </c>
-      <c r="B26" s="3" t="s">
+      <c r="E25" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="B26" t="s">
         <v>115</v>
       </c>
-      <c r="C26" s="3" t="s">
+      <c r="C26" t="s">
         <v>111</v>
       </c>
-      <c r="D26" s="3">
+      <c r="D26">
         <v>115</v>
       </c>
-      <c r="E26" s="3" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="5" t="s">
-        <v>108</v>
-      </c>
-      <c r="B27" s="3" t="s">
+      <c r="E26" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="B27" t="s">
         <v>116</v>
       </c>
-      <c r="C27" s="3" t="s">
+      <c r="C27" t="s">
         <v>111</v>
       </c>
-      <c r="D27" s="3">
+      <c r="D27">
         <v>98</v>
       </c>
-      <c r="E27" s="3" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A28" s="5" t="s">
-        <v>108</v>
-      </c>
-      <c r="B28" s="2" t="s">
+      <c r="E27" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="B28" t="s">
         <v>113</v>
       </c>
-      <c r="C28" s="3" t="s">
+      <c r="C28" t="s">
         <v>112</v>
       </c>
       <c r="D28">
         <v>1.264</v>
       </c>
       <c r="E28" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="B29" t="s">
+        <v>158</v>
+      </c>
+      <c r="C29" t="s">
+        <v>111</v>
+      </c>
+      <c r="D29">
+        <v>108</v>
+      </c>
+      <c r="E29" t="s">
         <v>56</v>
       </c>
     </row>
@@ -2377,22 +2428,22 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BBE77CEC-E9ED-4D7C-87C7-6AFD98461E9D}">
-  <dimension ref="A1:H27"/>
+  <dimension ref="A1:H28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C15" sqref="C15:C18"/>
+      <selection activeCell="H29" sqref="H29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="34.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="26.28515625" customWidth="1"/>
-    <col min="3" max="3" width="26.28515625" style="3" customWidth="1"/>
-    <col min="4" max="4" width="9.5703125" customWidth="1"/>
-    <col min="5" max="5" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.7109375" customWidth="1"/>
-    <col min="8" max="8" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="27.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="22.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
@@ -2402,7 +2453,7 @@
       <c r="B1" t="s">
         <v>40</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" t="s">
         <v>1</v>
       </c>
       <c r="D1" t="s">
@@ -2422,552 +2473,531 @@
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+      <c r="A2" t="s">
         <v>16</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" t="s">
         <v>65</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="E2" s="6" t="s">
+      <c r="D2" t="s">
+        <v>56</v>
+      </c>
+      <c r="E2" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="F2" s="6" t="s">
+      <c r="F2" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="G2" s="6" t="s">
+      <c r="G2" s="3" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
+      <c r="A3" t="s">
         <v>17</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" t="s">
         <v>66</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" t="s">
         <v>7</v>
       </c>
-      <c r="D3" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="E3" s="6" t="s">
+      <c r="D3" t="s">
+        <v>56</v>
+      </c>
+      <c r="E3" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="F3" s="6" t="s">
+      <c r="F3" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="G3" s="6" t="s">
+      <c r="G3" s="3" t="s">
         <v>130</v>
       </c>
-      <c r="H3" s="3"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
+      <c r="A4" t="s">
         <v>18</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" t="s">
         <v>67</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="E4" s="6" t="s">
+      <c r="D4" t="s">
+        <v>56</v>
+      </c>
+      <c r="E4" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="F4" s="6" t="s">
+      <c r="F4" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="G4" s="6" t="s">
+      <c r="G4" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="H4" s="3"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
+      <c r="A5" t="s">
         <v>19</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" t="s">
         <v>68</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="E5" s="6" t="s">
+      <c r="D5" t="s">
+        <v>56</v>
+      </c>
+      <c r="E5" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="F5" s="6" t="s">
+      <c r="F5" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="G5" s="6" t="s">
+      <c r="G5" s="3" t="s">
         <v>130</v>
       </c>
-      <c r="H5" s="3"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
+      <c r="A6" t="s">
         <v>20</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" t="s">
         <v>69</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C6" t="s">
         <v>10</v>
       </c>
-      <c r="D6" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="E6" s="6" t="s">
+      <c r="D6" t="s">
+        <v>56</v>
+      </c>
+      <c r="E6" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="F6" s="6" t="s">
+      <c r="F6" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="G6" s="6" t="s">
+      <c r="G6" s="3" t="s">
         <v>130</v>
       </c>
-      <c r="H6" s="3"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
+      <c r="A7" t="s">
         <v>21</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B7" t="s">
         <v>70</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="C7" t="s">
         <v>11</v>
       </c>
-      <c r="D7" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="E7" s="6" t="s">
+      <c r="D7" t="s">
+        <v>56</v>
+      </c>
+      <c r="E7" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="F7" s="6" t="s">
+      <c r="F7" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="G7" s="6" t="s">
+      <c r="G7" s="3" t="s">
         <v>130</v>
       </c>
-      <c r="H7" s="3"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
+      <c r="A8" t="s">
         <v>22</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B8" t="s">
         <v>71</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="C8" t="s">
         <v>12</v>
       </c>
-      <c r="D8" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="E8" s="6" t="s">
+      <c r="D8" t="s">
+        <v>56</v>
+      </c>
+      <c r="E8" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="F8" s="6" t="s">
+      <c r="F8" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="G8" s="6" t="s">
+      <c r="G8" s="3" t="s">
         <v>130</v>
       </c>
-      <c r="H8" s="3"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
+      <c r="A9" t="s">
         <v>23</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="B9" t="s">
         <v>72</v>
       </c>
-      <c r="C9" s="3" t="s">
+      <c r="C9" t="s">
         <v>13</v>
       </c>
-      <c r="D9" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="E9" s="6" t="s">
+      <c r="D9" t="s">
+        <v>56</v>
+      </c>
+      <c r="E9" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="F9" s="6" t="s">
+      <c r="F9" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="G9" s="6" t="s">
+      <c r="G9" s="3" t="s">
         <v>130</v>
       </c>
-      <c r="H9" s="3"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
+      <c r="A10" t="s">
         <v>24</v>
       </c>
-      <c r="B10" s="3" t="s">
+      <c r="B10" t="s">
         <v>73</v>
       </c>
-      <c r="C10" s="3" t="s">
+      <c r="C10" t="s">
         <v>14</v>
       </c>
-      <c r="D10" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="E10" s="6" t="s">
+      <c r="D10" t="s">
+        <v>56</v>
+      </c>
+      <c r="E10" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="F10" s="6" t="s">
+      <c r="F10" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="G10" s="6" t="s">
+      <c r="G10" s="3" t="s">
         <v>130</v>
       </c>
-      <c r="H10" s="3"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
+      <c r="A11" t="s">
         <v>25</v>
       </c>
-      <c r="B11" s="3" t="s">
+      <c r="B11" t="s">
         <v>74</v>
       </c>
-      <c r="C11" s="3" t="s">
+      <c r="C11" t="s">
         <v>15</v>
       </c>
-      <c r="D11" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="E11" s="6" t="s">
+      <c r="D11" t="s">
+        <v>56</v>
+      </c>
+      <c r="E11" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="F11" s="6" t="s">
+      <c r="F11" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="G11" s="6" t="s">
+      <c r="G11" s="3" t="s">
         <v>130</v>
       </c>
-      <c r="H11" s="3"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="2" t="s">
+      <c r="A12" t="s">
         <v>42</v>
       </c>
-      <c r="B12" s="3" t="s">
+      <c r="B12" t="s">
         <v>75</v>
       </c>
-      <c r="C12" s="3" t="s">
+      <c r="C12" t="s">
         <v>137</v>
       </c>
-      <c r="D12" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="E12" s="6" t="s">
+      <c r="D12" t="s">
+        <v>56</v>
+      </c>
+      <c r="E12" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="F12" s="6" t="s">
+      <c r="F12" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="G12" s="6" t="s">
+      <c r="G12" s="3" t="s">
         <v>130</v>
       </c>
-      <c r="H12" s="3"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="2" t="s">
+      <c r="A13" t="s">
         <v>43</v>
       </c>
-      <c r="B13" s="3" t="s">
+      <c r="B13" t="s">
         <v>76</v>
       </c>
-      <c r="C13" s="3" t="s">
+      <c r="C13" t="s">
         <v>138</v>
       </c>
-      <c r="D13" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="E13" s="6" t="s">
+      <c r="D13" t="s">
+        <v>56</v>
+      </c>
+      <c r="E13" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="F13" s="6" t="s">
+      <c r="F13" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="G13" s="6" t="s">
+      <c r="G13" s="3" t="s">
         <v>130</v>
       </c>
-      <c r="H13" s="3"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="2" t="s">
+      <c r="A14" t="s">
         <v>44</v>
       </c>
-      <c r="B14" s="3" t="s">
+      <c r="B14" t="s">
         <v>77</v>
       </c>
-      <c r="C14" s="3" t="s">
+      <c r="C14" t="s">
         <v>139</v>
       </c>
       <c r="D14" t="s">
         <v>56</v>
       </c>
-      <c r="E14" s="6" t="s">
+      <c r="E14" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="F14" s="6" t="s">
+      <c r="F14" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="G14" s="6" t="s">
+      <c r="G14" s="3" t="s">
         <v>130</v>
       </c>
-      <c r="H14" s="3"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>45</v>
       </c>
-      <c r="B15" s="3" t="s">
+      <c r="B15" t="s">
         <v>78</v>
       </c>
-      <c r="C15" s="3" t="s">
+      <c r="C15" t="s">
         <v>140</v>
       </c>
       <c r="D15" t="s">
         <v>56</v>
       </c>
-      <c r="E15" s="6" t="s">
+      <c r="E15" s="3" t="s">
         <v>121</v>
       </c>
-      <c r="F15" s="6" t="s">
+      <c r="F15" s="3" t="s">
         <v>122</v>
       </c>
-      <c r="G15" s="6" t="s">
+      <c r="G15" s="3" t="s">
         <v>130</v>
       </c>
-      <c r="H15" s="3"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>46</v>
       </c>
-      <c r="B16" s="3" t="s">
+      <c r="B16" t="s">
         <v>79</v>
       </c>
-      <c r="C16" s="3" t="s">
+      <c r="C16" t="s">
         <v>141</v>
       </c>
       <c r="D16" t="s">
         <v>56</v>
       </c>
-      <c r="E16" s="6" t="s">
+      <c r="E16" s="3" t="s">
         <v>121</v>
       </c>
-      <c r="F16" s="6" t="s">
+      <c r="F16" s="3" t="s">
         <v>122</v>
       </c>
-      <c r="G16" s="6" t="s">
+      <c r="G16" s="3" t="s">
         <v>130</v>
       </c>
-      <c r="H16" s="3"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>47</v>
       </c>
-      <c r="B17" s="3" t="s">
+      <c r="B17" t="s">
         <v>86</v>
       </c>
-      <c r="C17" s="3" t="s">
+      <c r="C17" t="s">
         <v>148</v>
       </c>
       <c r="D17" t="s">
         <v>55</v>
       </c>
-      <c r="E17" s="6" t="s">
+      <c r="E17" s="3" t="s">
         <v>121</v>
       </c>
-      <c r="F17" s="6" t="s">
+      <c r="F17" s="3" t="s">
         <v>122</v>
       </c>
-      <c r="G17" s="6" t="s">
+      <c r="G17" s="3" t="s">
         <v>128</v>
       </c>
-      <c r="H17" s="3"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>48</v>
       </c>
-      <c r="B18" s="3" t="s">
+      <c r="B18" t="s">
         <v>80</v>
       </c>
-      <c r="C18" s="3" t="s">
+      <c r="C18" t="s">
         <v>142</v>
       </c>
       <c r="D18" t="s">
         <v>56</v>
       </c>
-      <c r="E18" s="6" t="s">
+      <c r="E18" s="3" t="s">
         <v>121</v>
       </c>
-      <c r="F18" s="6" t="s">
+      <c r="F18" s="3" t="s">
         <v>122</v>
       </c>
-      <c r="G18" s="6" t="s">
+      <c r="G18" s="3" t="s">
         <v>129</v>
       </c>
-      <c r="H18" s="3"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>49</v>
       </c>
-      <c r="B19" s="3" t="s">
+      <c r="B19" t="s">
         <v>81</v>
       </c>
-      <c r="C19" s="3" t="s">
+      <c r="C19" t="s">
         <v>143</v>
       </c>
       <c r="D19" t="s">
         <v>56</v>
       </c>
-      <c r="E19" s="6" t="s">
+      <c r="E19" s="3" t="s">
         <v>123</v>
       </c>
-      <c r="F19" s="6" t="s">
+      <c r="F19" s="3" t="s">
         <v>124</v>
       </c>
-      <c r="G19" s="6" t="s">
+      <c r="G19" s="3" t="s">
         <v>130</v>
       </c>
-      <c r="H19" s="3"/>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>50</v>
       </c>
-      <c r="B20" s="3" t="s">
+      <c r="B20" t="s">
         <v>82</v>
       </c>
-      <c r="C20" s="3" t="s">
+      <c r="C20" t="s">
         <v>144</v>
       </c>
       <c r="D20" t="s">
         <v>56</v>
       </c>
-      <c r="E20" s="6" t="s">
+      <c r="E20" s="3" t="s">
         <v>123</v>
       </c>
-      <c r="F20" s="6" t="s">
+      <c r="F20" s="3" t="s">
         <v>124</v>
       </c>
-      <c r="G20" s="6" t="s">
+      <c r="G20" s="3" t="s">
         <v>130</v>
       </c>
-      <c r="H20" s="3"/>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>51</v>
       </c>
-      <c r="B21" s="3" t="s">
+      <c r="B21" t="s">
         <v>83</v>
       </c>
-      <c r="C21" s="3" t="s">
+      <c r="C21" t="s">
         <v>145</v>
       </c>
       <c r="D21" t="s">
         <v>56</v>
       </c>
-      <c r="E21" s="6" t="s">
+      <c r="E21" s="3" t="s">
         <v>123</v>
       </c>
-      <c r="F21" s="6" t="s">
+      <c r="F21" s="3" t="s">
         <v>124</v>
       </c>
-      <c r="G21" s="6" t="s">
+      <c r="G21" s="3" t="s">
         <v>130</v>
       </c>
-      <c r="H21" s="3"/>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>52</v>
       </c>
-      <c r="B22" s="3" t="s">
+      <c r="B22" t="s">
         <v>85</v>
       </c>
-      <c r="C22" s="3" t="s">
+      <c r="C22" t="s">
         <v>149</v>
       </c>
       <c r="D22" t="s">
         <v>55</v>
       </c>
-      <c r="E22" s="6" t="s">
+      <c r="E22" s="3" t="s">
         <v>123</v>
       </c>
-      <c r="F22" s="6" t="s">
+      <c r="F22" s="3" t="s">
         <v>124</v>
       </c>
-      <c r="G22" s="6" t="s">
+      <c r="G22" s="3" t="s">
         <v>128</v>
       </c>
-      <c r="H22" s="3"/>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>53</v>
       </c>
-      <c r="B23" s="3" t="s">
+      <c r="B23" t="s">
         <v>84</v>
       </c>
-      <c r="C23" s="3" t="s">
+      <c r="C23" t="s">
         <v>146</v>
       </c>
       <c r="D23" t="s">
         <v>56</v>
       </c>
-      <c r="E23" s="6" t="s">
+      <c r="E23" s="3" t="s">
         <v>123</v>
       </c>
-      <c r="F23" s="6" t="s">
+      <c r="F23" s="3" t="s">
         <v>124</v>
       </c>
-      <c r="G23" s="6" t="s">
+      <c r="G23" s="3" t="s">
         <v>129</v>
       </c>
-      <c r="H23" s="3"/>
-    </row>
-    <row r="24" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="3" t="s">
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
         <v>125</v>
       </c>
-      <c r="B24" s="3" t="s">
+      <c r="B24" t="s">
         <v>126</v>
       </c>
-      <c r="C24" s="3" t="s">
+      <c r="C24" t="s">
         <v>147</v>
       </c>
-      <c r="D24" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="E24" s="6" t="s">
+      <c r="D24" t="s">
+        <v>56</v>
+      </c>
+      <c r="E24" s="3" t="s">
         <v>123</v>
       </c>
-      <c r="F24" s="6" t="s">
+      <c r="F24" s="3" t="s">
         <v>127</v>
       </c>
-      <c r="G24" s="6" t="s">
+      <c r="G24" s="3" t="s">
         <v>130</v>
       </c>
     </row>
@@ -2978,19 +3008,19 @@
       <c r="B25" t="s">
         <v>115</v>
       </c>
-      <c r="D25" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="E25" s="6" t="s">
+      <c r="D25" t="s">
+        <v>56</v>
+      </c>
+      <c r="E25" s="3" t="s">
         <v>121</v>
       </c>
-      <c r="F25" s="6" t="s">
+      <c r="F25" s="3" t="s">
         <v>131</v>
       </c>
-      <c r="G25" s="6" t="s">
+      <c r="G25" s="3" t="s">
         <v>132</v>
       </c>
-      <c r="H25" s="3" t="s">
+      <c r="H25" t="s">
         <v>62</v>
       </c>
     </row>
@@ -3001,19 +3031,19 @@
       <c r="B26" t="s">
         <v>116</v>
       </c>
-      <c r="D26" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="E26" s="6" t="s">
+      <c r="D26" t="s">
+        <v>56</v>
+      </c>
+      <c r="E26" s="3" t="s">
         <v>123</v>
       </c>
-      <c r="F26" s="6" t="s">
+      <c r="F26" s="3" t="s">
         <v>131</v>
       </c>
-      <c r="G26" s="6" t="s">
+      <c r="G26" s="3" t="s">
         <v>132</v>
       </c>
-      <c r="H26" s="3" t="s">
+      <c r="H26" t="s">
         <v>63</v>
       </c>
     </row>
@@ -3024,20 +3054,43 @@
       <c r="B27" t="s">
         <v>114</v>
       </c>
-      <c r="D27" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="E27" s="6" t="s">
+      <c r="D27" t="s">
+        <v>56</v>
+      </c>
+      <c r="E27" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="F27" s="6" t="s">
+      <c r="F27" s="3" t="s">
         <v>131</v>
       </c>
-      <c r="G27" s="6" t="s">
+      <c r="G27" s="3" t="s">
         <v>130</v>
       </c>
-      <c r="H27" s="3" t="s">
+      <c r="H27" t="s">
         <v>64</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>157</v>
+      </c>
+      <c r="B28" t="s">
+        <v>158</v>
+      </c>
+      <c r="D28" t="s">
+        <v>56</v>
+      </c>
+      <c r="E28" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="F28" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="G28" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="H28" t="s">
+        <v>159</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
SE-2873 Extended to use notional cost
</commit_message>
<xml_diff>
--- a/examples/use-cases/valuation/data/lookthrough_data.xlsx
+++ b/examples/use-cases/valuation/data/lookthrough_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11113"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AndrewPoulter\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/steve/work/code/sample-notebooks/examples/use-cases/valuation/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBE33215-F025-4C51-8363-D3E1CEAE9E90}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{305D482E-92E9-514D-85C6-DDCC66C4B294}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{140D0F4F-AA5F-4E16-95A8-8F9F58C5F424}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="29040" windowHeight="15840" xr2:uid="{140D0F4F-AA5F-4E16-95A8-8F9F58C5F424}"/>
   </bookViews>
   <sheets>
     <sheet name="transactions" sheetId="3" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="540" uniqueCount="160">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="541" uniqueCount="162">
   <si>
     <t>date</t>
   </si>
@@ -517,6 +517,12 @@
   </si>
   <si>
     <t>USEquityFinancials</t>
+  </si>
+  <si>
+    <t>OpenContract</t>
+  </si>
+  <si>
+    <t>notional_amount</t>
   </si>
 </sst>
 </file>
@@ -524,7 +530,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -567,7 +573,7 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -895,29 +901,29 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33E4483A-D81C-486B-9469-6BB1913F7014}">
-  <dimension ref="A1:L22"/>
+  <dimension ref="A1:M22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L23" sqref="L23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M23" sqref="M23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="19.85546875" customWidth="1"/>
-    <col min="6" max="6" width="26.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="28.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="18.42578125" customWidth="1"/>
-    <col min="10" max="10" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="19.83203125" customWidth="1"/>
+    <col min="6" max="6" width="26.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="28.1640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.5" customWidth="1"/>
+    <col min="10" max="10" width="8.5" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="12" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="18.5703125" bestFit="1" customWidth="1"/>
-    <col min="13" max="14" width="9.28515625" customWidth="1"/>
+    <col min="12" max="12" width="18.5" bestFit="1" customWidth="1"/>
+    <col min="13" max="14" width="9.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>90</v>
       </c>
@@ -954,8 +960,11 @@
       <c r="L1" s="1" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M1" s="1" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>93</v>
       </c>
@@ -989,8 +998,11 @@
       <c r="L2">
         <v>291800</v>
       </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>94</v>
       </c>
@@ -1024,8 +1036,11 @@
       <c r="L3">
         <v>89815</v>
       </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>95</v>
       </c>
@@ -1059,8 +1074,11 @@
       <c r="L4">
         <v>90037.5</v>
       </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>96</v>
       </c>
@@ -1068,7 +1086,7 @@
         <v>107</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>92</v>
+        <v>160</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>107</v>
@@ -1092,10 +1110,13 @@
         <v>7469.99</v>
       </c>
       <c r="L5">
+        <v>50</v>
+      </c>
+      <c r="M5">
         <v>746999</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>97</v>
       </c>
@@ -1129,8 +1150,11 @@
       <c r="L6">
         <v>1300000</v>
       </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>98</v>
       </c>
@@ -1164,8 +1188,11 @@
       <c r="L7">
         <v>145050</v>
       </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>99</v>
       </c>
@@ -1199,8 +1226,11 @@
       <c r="L8">
         <v>49364.999999999993</v>
       </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>100</v>
       </c>
@@ -1234,8 +1264,11 @@
       <c r="L9">
         <v>363480</v>
       </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>101</v>
       </c>
@@ -1269,8 +1302,11 @@
       <c r="L10">
         <v>32840</v>
       </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>102</v>
       </c>
@@ -1304,8 +1340,11 @@
       <c r="L11">
         <v>700000</v>
       </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>103</v>
       </c>
@@ -1339,8 +1378,11 @@
       <c r="L12">
         <v>41967.5</v>
       </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>104</v>
       </c>
@@ -1374,8 +1416,11 @@
       <c r="L13">
         <v>64250</v>
       </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>105</v>
       </c>
@@ -1409,8 +1454,11 @@
       <c r="L14">
         <v>40733</v>
       </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>118</v>
       </c>
@@ -1444,8 +1492,11 @@
       <c r="L15">
         <v>686100</v>
       </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>119</v>
       </c>
@@ -1479,8 +1530,11 @@
       <c r="L16">
         <v>3955.0000000000005</v>
       </c>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>120</v>
       </c>
@@ -1514,8 +1568,11 @@
       <c r="L17">
         <v>1000000</v>
       </c>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>150</v>
       </c>
@@ -1549,8 +1606,11 @@
       <c r="L18">
         <v>5975</v>
       </c>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>151</v>
       </c>
@@ -1584,8 +1644,11 @@
       <c r="L19">
         <v>5700</v>
       </c>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>152</v>
       </c>
@@ -1619,8 +1682,11 @@
       <c r="L20">
         <v>4800</v>
       </c>
-    </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>153</v>
       </c>
@@ -1654,8 +1720,11 @@
       <c r="L21">
         <v>20000</v>
       </c>
-    </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>156</v>
       </c>
@@ -1692,6 +1761,9 @@
       <c r="L22">
         <f>K22*G22</f>
         <v>2650</v>
+      </c>
+      <c r="M22">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -1708,16 +1780,16 @@
       <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="20.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1734,7 +1806,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>108</v>
       </c>
@@ -1751,7 +1823,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>108</v>
       </c>
@@ -1768,7 +1840,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>108</v>
       </c>
@@ -1785,7 +1857,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>108</v>
       </c>
@@ -1802,7 +1874,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>108</v>
       </c>
@@ -1819,7 +1891,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>108</v>
       </c>
@@ -1836,7 +1908,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>108</v>
       </c>
@@ -1853,7 +1925,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>108</v>
       </c>
@@ -1870,7 +1942,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>108</v>
       </c>
@@ -1887,7 +1959,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
         <v>108</v>
       </c>
@@ -1915,20 +1987,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E615609-E297-47FD-9AAE-07E524F332F5}">
   <dimension ref="A1:E29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="27.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="6" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1945,7 +2017,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>108</v>
       </c>
@@ -1962,7 +2034,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>108</v>
       </c>
@@ -1979,7 +2051,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>108</v>
       </c>
@@ -1996,7 +2068,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>108</v>
       </c>
@@ -2013,7 +2085,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>108</v>
       </c>
@@ -2030,7 +2102,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>108</v>
       </c>
@@ -2047,7 +2119,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>108</v>
       </c>
@@ -2064,7 +2136,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>108</v>
       </c>
@@ -2081,7 +2153,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>108</v>
       </c>
@@ -2098,7 +2170,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
         <v>108</v>
       </c>
@@ -2115,7 +2187,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
         <v>108</v>
       </c>
@@ -2132,7 +2204,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
         <v>108</v>
       </c>
@@ -2149,7 +2221,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
         <v>108</v>
       </c>
@@ -2166,7 +2238,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
         <v>108</v>
       </c>
@@ -2183,7 +2255,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
         <v>108</v>
       </c>
@@ -2200,7 +2272,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
         <v>108</v>
       </c>
@@ -2217,7 +2289,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
         <v>108</v>
       </c>
@@ -2234,7 +2306,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
         <v>108</v>
       </c>
@@ -2251,7 +2323,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
         <v>108</v>
       </c>
@@ -2268,7 +2340,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
         <v>108</v>
       </c>
@@ -2285,7 +2357,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
         <v>108</v>
       </c>
@@ -2302,7 +2374,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
         <v>108</v>
       </c>
@@ -2319,7 +2391,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
         <v>108</v>
       </c>
@@ -2336,7 +2408,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
         <v>108</v>
       </c>
@@ -2353,7 +2425,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
         <v>108</v>
       </c>
@@ -2370,7 +2442,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="s">
         <v>108</v>
       </c>
@@ -2387,7 +2459,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28" s="2" t="s">
         <v>108</v>
       </c>
@@ -2404,7 +2476,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29" s="2" t="s">
         <v>108</v>
       </c>
@@ -2434,19 +2506,19 @@
       <selection activeCell="H29" sqref="H29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="27.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="28.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="27.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.5" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="16" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="22.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="22.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -2472,7 +2544,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>16</v>
       </c>
@@ -2495,7 +2567,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>17</v>
       </c>
@@ -2518,7 +2590,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>18</v>
       </c>
@@ -2541,7 +2613,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>19</v>
       </c>
@@ -2564,7 +2636,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>20</v>
       </c>
@@ -2587,7 +2659,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>21</v>
       </c>
@@ -2610,7 +2682,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>22</v>
       </c>
@@ -2633,7 +2705,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>23</v>
       </c>
@@ -2656,7 +2728,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>24</v>
       </c>
@@ -2679,7 +2751,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>25</v>
       </c>
@@ -2702,7 +2774,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>42</v>
       </c>
@@ -2725,7 +2797,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>43</v>
       </c>
@@ -2748,7 +2820,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>44</v>
       </c>
@@ -2771,7 +2843,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>45</v>
       </c>
@@ -2794,7 +2866,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>46</v>
       </c>
@@ -2817,7 +2889,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>47</v>
       </c>
@@ -2840,7 +2912,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>48</v>
       </c>
@@ -2863,7 +2935,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>49</v>
       </c>
@@ -2886,7 +2958,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>50</v>
       </c>
@@ -2909,7 +2981,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>51</v>
       </c>
@@ -2932,7 +3004,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>52</v>
       </c>
@@ -2955,7 +3027,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>53</v>
       </c>
@@ -2978,7 +3050,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>125</v>
       </c>
@@ -3001,7 +3073,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>133</v>
       </c>
@@ -3024,7 +3096,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>134</v>
       </c>
@@ -3047,7 +3119,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>135</v>
       </c>
@@ -3070,7 +3142,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>157</v>
       </c>

</xml_diff>

<commit_message>
Create reqired property definition
</commit_message>
<xml_diff>
--- a/examples/use-cases/valuation/data/lookthrough_data.xlsx
+++ b/examples/use-cases/valuation/data/lookthrough_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/steve/work/code/sample-notebooks/examples/use-cases/valuation/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9400023-2C0A-144C-8002-DDD267600921}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1EC1928-1802-7C42-A9AE-C27E08606BBB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="20300" xr2:uid="{140D0F4F-AA5F-4E16-95A8-8F9F58C5F424}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="551" uniqueCount="165">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="546" uniqueCount="165">
   <si>
     <t>date</t>
   </si>
@@ -501,9 +501,6 @@
     <t>FundsIn</t>
   </si>
   <si>
-    <t>cash_id</t>
-  </si>
-  <si>
     <t>txnid_0021</t>
   </si>
   <si>
@@ -532,6 +529,9 @@
   </si>
   <si>
     <t>txnid_0004a</t>
+  </si>
+  <si>
+    <t>strategy</t>
   </si>
 </sst>
 </file>
@@ -913,7 +913,7 @@
   <dimension ref="A1:M23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+      <selection activeCell="I7" sqref="I7:I24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -958,7 +958,7 @@
         <v>40</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>154</v>
+        <v>164</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>39</v>
@@ -970,7 +970,7 @@
         <v>60</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.2">
@@ -1089,13 +1089,13 @@
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>106</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>106</v>
@@ -1113,7 +1113,7 @@
         <v>87</v>
       </c>
       <c r="I5" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="J5" s="1" t="s">
         <v>56</v>
@@ -1130,13 +1130,13 @@
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>106</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>106</v>
@@ -1154,7 +1154,7 @@
         <v>87</v>
       </c>
       <c r="I6" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="J6" s="1" t="s">
         <v>56</v>
@@ -1191,9 +1191,6 @@
       <c r="G7" s="1">
         <v>1300000</v>
       </c>
-      <c r="I7" t="s">
-        <v>56</v>
-      </c>
       <c r="J7" s="1" t="s">
         <v>56</v>
       </c>
@@ -1381,9 +1378,6 @@
       <c r="G12" s="1">
         <v>700000</v>
       </c>
-      <c r="I12" t="s">
-        <v>56</v>
-      </c>
       <c r="J12" s="1" t="s">
         <v>56</v>
       </c>
@@ -1414,7 +1408,7 @@
         <v>107</v>
       </c>
       <c r="F13" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="G13" s="1">
         <v>250</v>
@@ -1452,7 +1446,7 @@
         <v>107</v>
       </c>
       <c r="F14" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="G14" s="1">
         <v>1000</v>
@@ -1490,7 +1484,7 @@
         <v>107</v>
       </c>
       <c r="F15" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="G15" s="1">
         <v>100</v>
@@ -1609,9 +1603,6 @@
       <c r="G18" s="1">
         <v>1000000</v>
       </c>
-      <c r="I18" t="s">
-        <v>56</v>
-      </c>
       <c r="J18" s="1" t="s">
         <v>56</v>
       </c>
@@ -1761,9 +1752,6 @@
       <c r="G22" s="1">
         <v>20000</v>
       </c>
-      <c r="I22" t="s">
-        <v>56</v>
-      </c>
       <c r="J22" s="1" t="s">
         <v>56</v>
       </c>
@@ -1779,7 +1767,7 @@
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B23" s="2" t="s">
         <v>106</v>
@@ -1800,10 +1788,7 @@
         <v>25</v>
       </c>
       <c r="H23" t="s">
-        <v>157</v>
-      </c>
-      <c r="I23" t="s">
-        <v>56</v>
+        <v>156</v>
       </c>
       <c r="J23" s="1" t="s">
         <v>56</v>
@@ -2534,7 +2519,7 @@
         <v>107</v>
       </c>
       <c r="B29" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C29" t="s">
         <v>110</v>
@@ -3197,10 +3182,10 @@
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
+        <v>155</v>
+      </c>
+      <c r="B28" t="s">
         <v>156</v>
-      </c>
-      <c r="B28" t="s">
-        <v>157</v>
       </c>
       <c r="D28" t="s">
         <v>56</v>
@@ -3215,7 +3200,7 @@
         <v>129</v>
       </c>
       <c r="H28" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
   </sheetData>

</xml_diff>